<commit_message>
combobox from enum with localization
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\AppResponsiveMenu\lang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63267F4F-4C07-497A-AA00-DF4D6077D53A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2F26C0-38B1-4899-B100-A8C55ABBBF96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="1350" windowWidth="20280" windowHeight="12510" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
+    <workbookView xWindow="-21390" yWindow="2115" windowWidth="20280" windowHeight="12510" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="5" r:id="rId1"/>
@@ -8068,8 +8068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414197DE-5D7D-415C-BB9E-1CF1298E8AD7}">
   <dimension ref="A1:C864"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A845" workbookViewId="0">
-      <selection activeCell="A865" sqref="A865"/>
+    <sheetView tabSelected="1" topLeftCell="A840" workbookViewId="0">
+      <selection activeCell="A865" sqref="A865:XFD865"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
monitoring settings view finished
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2F26C0-38B1-4899-B100-A8C55ABBBF96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4CE564-1B68-4742-A14A-F4385080FCD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21390" yWindow="2115" windowWidth="20280" windowHeight="12510" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
+    <workbookView xWindow="-22470" yWindow="1770" windowWidth="20280" windowHeight="12765" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2591" uniqueCount="2541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="2544">
   <si>
     <t>Name</t>
   </si>
@@ -7663,6 +7663,15 @@
   </si>
   <si>
     <t>Отзывчивый</t>
+  </si>
+  <si>
+    <t>SID_Rtu_Moni_Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTU  &lt;{{0}}&gt; Monitoring Settings </t>
+  </si>
+  <si>
+    <t>RTU  &lt;{{0}}&gt;  Настройки мониторинга</t>
   </si>
 </sst>
 </file>
@@ -8066,10 +8075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414197DE-5D7D-415C-BB9E-1CF1298E8AD7}">
-  <dimension ref="A1:C864"/>
+  <dimension ref="A1:C865"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A840" workbookViewId="0">
-      <selection activeCell="A865" sqref="A865:XFD865"/>
+    <sheetView tabSelected="1" topLeftCell="A849" workbookViewId="0">
+      <selection activeCell="A865" sqref="A865"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17570,6 +17579,17 @@
       </c>
       <c r="C864" t="s">
         <v>2540</v>
+      </c>
+    </row>
+    <row r="865" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A865" t="s">
+        <v>2541</v>
+      </c>
+      <c r="B865" t="s">
+        <v>2542</v>
+      </c>
+      <c r="C865" t="s">
+        <v>2543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
experiment 2 - three media ports
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4CE564-1B68-4742-A14A-F4385080FCD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4553C4-AD7C-4907-9B78-AA7C7653173E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22470" yWindow="1770" windowWidth="20280" windowHeight="12765" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="2544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="2555">
   <si>
     <t>Name</t>
   </si>
@@ -7673,18 +7673,58 @@
   <si>
     <t>RTU  &lt;{{0}}&gt;  Настройки мониторинга</t>
   </si>
+  <si>
+    <t>SID_saving_frequency</t>
+  </si>
+  <si>
+    <t>SID_measurement_frequency</t>
+  </si>
+  <si>
+    <t>measurement frequency</t>
+  </si>
+  <si>
+    <t>saving frequency</t>
+  </si>
+  <si>
+    <t>частота измерений</t>
+  </si>
+  <si>
+    <t>частота сохранения</t>
+  </si>
+  <si>
+    <t>SID_Cycle_full_time_sec</t>
+  </si>
+  <si>
+    <t>Cycle full time {{0}} sec</t>
+  </si>
+  <si>
+    <t>Полное время цикла {{0}} сек</t>
+  </si>
+  <si>
+    <t>SID_Auto</t>
+  </si>
+  <si>
+    <t>Авто</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -7707,8 +7747,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -8075,10 +8118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414197DE-5D7D-415C-BB9E-1CF1298E8AD7}">
-  <dimension ref="A1:C865"/>
+  <dimension ref="A1:C869"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A849" workbookViewId="0">
-      <selection activeCell="A865" sqref="A865"/>
+    <sheetView tabSelected="1" topLeftCell="A851" workbookViewId="0">
+      <selection activeCell="C870" sqref="C870"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17592,6 +17635,50 @@
         <v>2543</v>
       </c>
     </row>
+    <row r="866" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A866" t="s">
+        <v>2545</v>
+      </c>
+      <c r="B866" s="1" t="s">
+        <v>2546</v>
+      </c>
+      <c r="C866" t="s">
+        <v>2548</v>
+      </c>
+    </row>
+    <row r="867" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A867" t="s">
+        <v>2544</v>
+      </c>
+      <c r="B867" s="1" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C867" t="s">
+        <v>2549</v>
+      </c>
+    </row>
+    <row r="868" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A868" t="s">
+        <v>2550</v>
+      </c>
+      <c r="B868" t="s">
+        <v>2551</v>
+      </c>
+      <c r="C868" t="s">
+        <v>2552</v>
+      </c>
+    </row>
+    <row r="869" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A869" s="1" t="s">
+        <v>2553</v>
+      </c>
+      <c r="B869" t="s">
+        <v>227</v>
+      </c>
+      <c r="C869" t="s">
+        <v>2554</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C4 A6:C6 A8 A10">
     <cfRule type="containsBlanks" dxfId="0" priority="2">
@@ -17599,6 +17686,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17616,264 +17704,264 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
login error are displayed within login component
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4553C4-AD7C-4907-9B78-AA7C7653173E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBE3BA7-6DED-4762-8F40-387B65190F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22470" yWindow="1770" windowWidth="20280" windowHeight="12765" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
+    <workbookView xWindow="-21690" yWindow="1500" windowWidth="20280" windowHeight="12765" xr2:uid="{A7D3CB50-0A18-4D34-8249-9890304C4FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2606" uniqueCount="2555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2609" uniqueCount="2558">
   <si>
     <t>Name</t>
   </si>
@@ -6744,12 +6744,6 @@
     <t>SID_User_with_the_same_name_is_registered_on_another_PC</t>
   </si>
   <si>
-    <t>User with the same name is registered on another PC</t>
-  </si>
-  <si>
-    <t>Пользователь с таким именем подключился за другим PC</t>
-  </si>
-  <si>
     <t>SID_Users</t>
   </si>
   <si>
@@ -7705,6 +7699,21 @@
   </si>
   <si>
     <t>Авто</t>
+  </si>
+  <si>
+    <t>User with the same name is registered from another device</t>
+  </si>
+  <si>
+    <t>Пользователь с таким именем подключился с другого устройства</t>
+  </si>
+  <si>
+    <t>SID_This_user_has_no_right_to_start_Web_Client</t>
+  </si>
+  <si>
+    <t>This user has no right to start Web Client</t>
+  </si>
+  <si>
+    <t>Данный пользователь не имеет прав на запуск ПО Fibertest WebClient</t>
   </si>
 </sst>
 </file>
@@ -8118,10 +8127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{414197DE-5D7D-415C-BB9E-1CF1298E8AD7}">
-  <dimension ref="A1:C869"/>
+  <dimension ref="A1:C870"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A851" workbookViewId="0">
-      <selection activeCell="C870" sqref="C870"/>
+    <sheetView tabSelected="1" topLeftCell="A738" workbookViewId="0">
+      <selection activeCell="C757" sqref="C757"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8147,10 +8156,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>2309</v>
+        <v>2307</v>
       </c>
       <c r="C2" t="s">
-        <v>2310</v>
+        <v>2308</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -8158,10 +8167,10 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>2311</v>
+        <v>2309</v>
       </c>
       <c r="C3" t="s">
-        <v>2312</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -8213,10 +8222,10 @@
         <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>2313</v>
+        <v>2311</v>
       </c>
       <c r="C8" t="s">
-        <v>2314</v>
+        <v>2312</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -8235,10 +8244,10 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>2315</v>
+        <v>2313</v>
       </c>
       <c r="C10" t="s">
-        <v>2316</v>
+        <v>2314</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -8268,10 +8277,10 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>2317</v>
+        <v>2315</v>
       </c>
       <c r="C13" t="s">
-        <v>2318</v>
+        <v>2316</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -8290,10 +8299,10 @@
         <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>2319</v>
+        <v>2317</v>
       </c>
       <c r="C15" t="s">
-        <v>2320</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -8301,10 +8310,10 @@
         <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>2321</v>
+        <v>2319</v>
       </c>
       <c r="C16" t="s">
-        <v>2322</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -8312,10 +8321,10 @@
         <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>2323</v>
+        <v>2321</v>
       </c>
       <c r="C17" t="s">
-        <v>2324</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -8323,10 +8332,10 @@
         <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>2325</v>
+        <v>2323</v>
       </c>
       <c r="C18" t="s">
-        <v>2326</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -8334,10 +8343,10 @@
         <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>2327</v>
+        <v>2325</v>
       </c>
       <c r="C19" t="s">
-        <v>2328</v>
+        <v>2326</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -8345,10 +8354,10 @@
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>2329</v>
+        <v>2327</v>
       </c>
       <c r="C20" t="s">
-        <v>2330</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -8356,10 +8365,10 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>2331</v>
+        <v>2329</v>
       </c>
       <c r="C21" t="s">
-        <v>2332</v>
+        <v>2330</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -8367,10 +8376,10 @@
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>2333</v>
+        <v>2331</v>
       </c>
       <c r="C22" t="s">
-        <v>2334</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -8378,10 +8387,10 @@
         <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>2335</v>
+        <v>2333</v>
       </c>
       <c r="C23" t="s">
-        <v>2336</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -8389,10 +8398,10 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>2337</v>
+        <v>2335</v>
       </c>
       <c r="C24" t="s">
-        <v>2338</v>
+        <v>2336</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -8400,10 +8409,10 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>2339</v>
+        <v>2337</v>
       </c>
       <c r="C25" t="s">
-        <v>2340</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -8411,10 +8420,10 @@
         <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>2341</v>
+        <v>2339</v>
       </c>
       <c r="C26" t="s">
-        <v>2342</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -8422,10 +8431,10 @@
         <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>2343</v>
+        <v>2341</v>
       </c>
       <c r="C27" t="s">
-        <v>2344</v>
+        <v>2342</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -8433,10 +8442,10 @@
         <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>2345</v>
+        <v>2343</v>
       </c>
       <c r="C28" t="s">
-        <v>2346</v>
+        <v>2344</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -8444,10 +8453,10 @@
         <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>2347</v>
+        <v>2345</v>
       </c>
       <c r="C29" t="s">
-        <v>2348</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -8455,10 +8464,10 @@
         <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>2349</v>
+        <v>2347</v>
       </c>
       <c r="C30" t="s">
-        <v>2350</v>
+        <v>2348</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -8466,10 +8475,10 @@
         <v>54</v>
       </c>
       <c r="B31" t="s">
-        <v>2351</v>
+        <v>2349</v>
       </c>
       <c r="C31" t="s">
-        <v>2352</v>
+        <v>2350</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -8477,10 +8486,10 @@
         <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>2353</v>
+        <v>2351</v>
       </c>
       <c r="C32" t="s">
-        <v>2354</v>
+        <v>2352</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -8631,10 +8640,10 @@
         <v>95</v>
       </c>
       <c r="B46" t="s">
-        <v>2355</v>
+        <v>2353</v>
       </c>
       <c r="C46" t="s">
-        <v>2356</v>
+        <v>2354</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -8961,10 +8970,10 @@
         <v>183</v>
       </c>
       <c r="B76" t="s">
-        <v>2357</v>
+        <v>2355</v>
       </c>
       <c r="C76" t="s">
-        <v>2358</v>
+        <v>2356</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -9203,10 +9212,10 @@
         <v>244</v>
       </c>
       <c r="B98" t="s">
-        <v>2359</v>
+        <v>2357</v>
       </c>
       <c r="C98" t="s">
-        <v>2360</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -9280,10 +9289,10 @@
         <v>263</v>
       </c>
       <c r="B105" t="s">
-        <v>2361</v>
+        <v>2359</v>
       </c>
       <c r="C105" t="s">
-        <v>2362</v>
+        <v>2360</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -9313,10 +9322,10 @@
         <v>270</v>
       </c>
       <c r="B108" t="s">
-        <v>2363</v>
+        <v>2361</v>
       </c>
       <c r="C108" t="s">
-        <v>2364</v>
+        <v>2362</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -9412,10 +9421,10 @@
         <v>294</v>
       </c>
       <c r="B117" t="s">
-        <v>2365</v>
+        <v>2363</v>
       </c>
       <c r="C117" t="s">
-        <v>2366</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -9445,10 +9454,10 @@
         <v>301</v>
       </c>
       <c r="B120" t="s">
-        <v>2367</v>
+        <v>2365</v>
       </c>
       <c r="C120" t="s">
-        <v>2368</v>
+        <v>2366</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -9467,10 +9476,10 @@
         <v>305</v>
       </c>
       <c r="B122" t="s">
-        <v>2369</v>
+        <v>2367</v>
       </c>
       <c r="C122" t="s">
-        <v>2370</v>
+        <v>2368</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -9500,10 +9509,10 @@
         <v>311</v>
       </c>
       <c r="B125" t="s">
-        <v>2371</v>
+        <v>2369</v>
       </c>
       <c r="C125" t="s">
-        <v>2372</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -9566,10 +9575,10 @@
         <v>327</v>
       </c>
       <c r="B131" t="s">
-        <v>2373</v>
+        <v>2371</v>
       </c>
       <c r="C131" t="s">
-        <v>2374</v>
+        <v>2372</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -9588,10 +9597,10 @@
         <v>331</v>
       </c>
       <c r="B133" t="s">
-        <v>2375</v>
+        <v>2373</v>
       </c>
       <c r="C133" t="s">
-        <v>2376</v>
+        <v>2374</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -9676,10 +9685,10 @@
         <v>352</v>
       </c>
       <c r="B141" t="s">
-        <v>2377</v>
+        <v>2375</v>
       </c>
       <c r="C141" t="s">
-        <v>2378</v>
+        <v>2376</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -9720,10 +9729,10 @@
         <v>362</v>
       </c>
       <c r="B145" t="s">
-        <v>2379</v>
+        <v>2377</v>
       </c>
       <c r="C145" t="s">
-        <v>2380</v>
+        <v>2378</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -9764,10 +9773,10 @@
         <v>372</v>
       </c>
       <c r="B149" t="s">
-        <v>2381</v>
+        <v>2379</v>
       </c>
       <c r="C149" t="s">
-        <v>2382</v>
+        <v>2380</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -9841,10 +9850,10 @@
         <v>391</v>
       </c>
       <c r="B156" t="s">
-        <v>2383</v>
+        <v>2381</v>
       </c>
       <c r="C156" t="s">
-        <v>2383</v>
+        <v>2381</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -9896,10 +9905,10 @@
         <v>404</v>
       </c>
       <c r="B161" t="s">
-        <v>2384</v>
+        <v>2382</v>
       </c>
       <c r="C161" t="s">
-        <v>2385</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -10105,10 +10114,10 @@
         <v>459</v>
       </c>
       <c r="B180" t="s">
-        <v>2386</v>
+        <v>2384</v>
       </c>
       <c r="C180" t="s">
-        <v>2387</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -10127,10 +10136,10 @@
         <v>463</v>
       </c>
       <c r="B182" t="s">
-        <v>2388</v>
+        <v>2386</v>
       </c>
       <c r="C182" t="s">
-        <v>2389</v>
+        <v>2387</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
@@ -10149,10 +10158,10 @@
         <v>467</v>
       </c>
       <c r="B184" t="s">
-        <v>2390</v>
+        <v>2388</v>
       </c>
       <c r="C184" t="s">
-        <v>2391</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
@@ -10160,10 +10169,10 @@
         <v>468</v>
       </c>
       <c r="B185" t="s">
-        <v>2392</v>
+        <v>2390</v>
       </c>
       <c r="C185" t="s">
-        <v>2393</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
@@ -10259,10 +10268,10 @@
         <v>493</v>
       </c>
       <c r="B194" t="s">
-        <v>2394</v>
+        <v>2392</v>
       </c>
       <c r="C194" t="s">
-        <v>2395</v>
+        <v>2393</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -10281,10 +10290,10 @@
         <v>497</v>
       </c>
       <c r="B196" t="s">
-        <v>2396</v>
+        <v>2394</v>
       </c>
       <c r="C196" t="s">
-        <v>2397</v>
+        <v>2395</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -11084,10 +11093,10 @@
         <v>707</v>
       </c>
       <c r="B269" t="s">
-        <v>2398</v>
+        <v>2396</v>
       </c>
       <c r="C269" t="s">
-        <v>2399</v>
+        <v>2397</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -11117,10 +11126,10 @@
         <v>714</v>
       </c>
       <c r="B272" t="s">
-        <v>2400</v>
+        <v>2398</v>
       </c>
       <c r="C272" t="s">
-        <v>2401</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -11161,10 +11170,10 @@
         <v>724</v>
       </c>
       <c r="B276" t="s">
-        <v>2402</v>
+        <v>2400</v>
       </c>
       <c r="C276" t="s">
-        <v>2403</v>
+        <v>2401</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -11238,10 +11247,10 @@
         <v>743</v>
       </c>
       <c r="B283" t="s">
-        <v>2404</v>
+        <v>2402</v>
       </c>
       <c r="C283" t="s">
-        <v>2405</v>
+        <v>2403</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -11491,10 +11500,10 @@
         <v>808</v>
       </c>
       <c r="B306" t="s">
-        <v>2406</v>
+        <v>2404</v>
       </c>
       <c r="C306" t="s">
-        <v>2407</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
@@ -11645,10 +11654,10 @@
         <v>847</v>
       </c>
       <c r="B320" t="s">
-        <v>2408</v>
+        <v>2406</v>
       </c>
       <c r="C320" t="s">
-        <v>2409</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -11711,10 +11720,10 @@
         <v>863</v>
       </c>
       <c r="B326" t="s">
-        <v>2410</v>
+        <v>2408</v>
       </c>
       <c r="C326" t="s">
-        <v>2411</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
@@ -11986,10 +11995,10 @@
         <v>935</v>
       </c>
       <c r="B351" t="s">
-        <v>2412</v>
+        <v>2410</v>
       </c>
       <c r="C351" t="s">
-        <v>2413</v>
+        <v>2411</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
@@ -12272,10 +12281,10 @@
         <v>1011</v>
       </c>
       <c r="B377" t="s">
-        <v>2414</v>
+        <v>2412</v>
       </c>
       <c r="C377" t="s">
-        <v>2415</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
@@ -12382,10 +12391,10 @@
         <v>1039</v>
       </c>
       <c r="B387" t="s">
-        <v>2416</v>
+        <v>2414</v>
       </c>
       <c r="C387" t="s">
-        <v>2417</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
@@ -12393,10 +12402,10 @@
         <v>1040</v>
       </c>
       <c r="B388" t="s">
-        <v>2418</v>
+        <v>2416</v>
       </c>
       <c r="C388" t="s">
-        <v>2419</v>
+        <v>2417</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
@@ -12437,10 +12446,10 @@
         <v>1050</v>
       </c>
       <c r="B392" t="s">
-        <v>2420</v>
+        <v>2418</v>
       </c>
       <c r="C392" t="s">
-        <v>2421</v>
+        <v>2419</v>
       </c>
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
@@ -12734,10 +12743,10 @@
         <v>1127</v>
       </c>
       <c r="B419" t="s">
-        <v>2422</v>
+        <v>2420</v>
       </c>
       <c r="C419" t="s">
-        <v>2423</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
@@ -12943,10 +12952,10 @@
         <v>1180</v>
       </c>
       <c r="B438" t="s">
-        <v>2424</v>
+        <v>2422</v>
       </c>
       <c r="C438" t="s">
-        <v>2425</v>
+        <v>2423</v>
       </c>
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.25">
@@ -12976,10 +12985,10 @@
         <v>1187</v>
       </c>
       <c r="B441" t="s">
-        <v>2426</v>
+        <v>2424</v>
       </c>
       <c r="C441" t="s">
-        <v>2427</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.25">
@@ -13020,10 +13029,10 @@
         <v>1197</v>
       </c>
       <c r="B445" t="s">
-        <v>2428</v>
+        <v>2426</v>
       </c>
       <c r="C445" t="s">
-        <v>2429</v>
+        <v>2427</v>
       </c>
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.25">
@@ -13042,10 +13051,10 @@
         <v>1201</v>
       </c>
       <c r="B447" t="s">
-        <v>2430</v>
+        <v>2428</v>
       </c>
       <c r="C447" t="s">
-        <v>2431</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
@@ -13119,10 +13128,10 @@
         <v>1220</v>
       </c>
       <c r="B454" t="s">
-        <v>2432</v>
+        <v>2430</v>
       </c>
       <c r="C454" t="s">
-        <v>2433</v>
+        <v>2431</v>
       </c>
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.25">
@@ -13130,10 +13139,10 @@
         <v>1221</v>
       </c>
       <c r="B455" t="s">
-        <v>2434</v>
+        <v>2432</v>
       </c>
       <c r="C455" t="s">
-        <v>2435</v>
+        <v>2433</v>
       </c>
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.25">
@@ -13141,10 +13150,10 @@
         <v>1222</v>
       </c>
       <c r="B456" t="s">
-        <v>2436</v>
+        <v>2434</v>
       </c>
       <c r="C456" t="s">
-        <v>2437</v>
+        <v>2435</v>
       </c>
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.25">
@@ -13174,10 +13183,10 @@
         <v>1229</v>
       </c>
       <c r="B459" t="s">
-        <v>2438</v>
+        <v>2436</v>
       </c>
       <c r="C459" t="s">
-        <v>2439</v>
+        <v>2437</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.25">
@@ -13185,10 +13194,10 @@
         <v>1230</v>
       </c>
       <c r="B460" t="s">
-        <v>2440</v>
+        <v>2438</v>
       </c>
       <c r="C460" t="s">
-        <v>2441</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.25">
@@ -13229,10 +13238,10 @@
         <v>1240</v>
       </c>
       <c r="B464" t="s">
-        <v>2442</v>
+        <v>2440</v>
       </c>
       <c r="C464" t="s">
-        <v>2443</v>
+        <v>2441</v>
       </c>
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.25">
@@ -13251,10 +13260,10 @@
         <v>1244</v>
       </c>
       <c r="B466" t="s">
-        <v>2444</v>
+        <v>2442</v>
       </c>
       <c r="C466" t="s">
-        <v>2445</v>
+        <v>2443</v>
       </c>
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.25">
@@ -13295,10 +13304,10 @@
         <v>1254</v>
       </c>
       <c r="B470" t="s">
-        <v>2446</v>
+        <v>2444</v>
       </c>
       <c r="C470" t="s">
-        <v>2446</v>
+        <v>2444</v>
       </c>
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.25">
@@ -13581,10 +13590,10 @@
         <v>1328</v>
       </c>
       <c r="B496" t="s">
-        <v>2447</v>
+        <v>2445</v>
       </c>
       <c r="C496" t="s">
-        <v>2448</v>
+        <v>2446</v>
       </c>
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.25">
@@ -13746,10 +13755,10 @@
         <v>1371</v>
       </c>
       <c r="B511" t="s">
-        <v>2449</v>
+        <v>2447</v>
       </c>
       <c r="C511" t="s">
-        <v>2449</v>
+        <v>2447</v>
       </c>
     </row>
     <row r="512" spans="1:3" x14ac:dyDescent="0.25">
@@ -13812,10 +13821,10 @@
         <v>1387</v>
       </c>
       <c r="B517" t="s">
-        <v>2450</v>
+        <v>2448</v>
       </c>
       <c r="C517" t="s">
-        <v>2450</v>
+        <v>2448</v>
       </c>
     </row>
     <row r="518" spans="1:3" x14ac:dyDescent="0.25">
@@ -13911,10 +13920,10 @@
         <v>1412</v>
       </c>
       <c r="B526" t="s">
-        <v>2451</v>
+        <v>2449</v>
       </c>
       <c r="C526" t="s">
-        <v>2452</v>
+        <v>2450</v>
       </c>
     </row>
     <row r="527" spans="1:3" x14ac:dyDescent="0.25">
@@ -13922,10 +13931,10 @@
         <v>1413</v>
       </c>
       <c r="B527" t="s">
-        <v>2453</v>
+        <v>2451</v>
       </c>
       <c r="C527" t="s">
-        <v>2454</v>
+        <v>2452</v>
       </c>
     </row>
     <row r="528" spans="1:3" x14ac:dyDescent="0.25">
@@ -13955,10 +13964,10 @@
         <v>1420</v>
       </c>
       <c r="B530" t="s">
-        <v>2455</v>
+        <v>2453</v>
       </c>
       <c r="C530" t="s">
-        <v>2456</v>
+        <v>2454</v>
       </c>
     </row>
     <row r="531" spans="1:3" x14ac:dyDescent="0.25">
@@ -14021,10 +14030,10 @@
         <v>1433</v>
       </c>
       <c r="B536" t="s">
-        <v>2457</v>
+        <v>2455</v>
       </c>
       <c r="C536" t="s">
-        <v>2457</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="537" spans="1:3" x14ac:dyDescent="0.25">
@@ -14032,10 +14041,10 @@
         <v>1434</v>
       </c>
       <c r="B537" t="s">
-        <v>2458</v>
+        <v>2456</v>
       </c>
       <c r="C537" t="s">
-        <v>2458</v>
+        <v>2456</v>
       </c>
     </row>
     <row r="538" spans="1:3" x14ac:dyDescent="0.25">
@@ -14197,10 +14206,10 @@
         <v>1477</v>
       </c>
       <c r="B552" t="s">
-        <v>2459</v>
+        <v>2457</v>
       </c>
       <c r="C552" t="s">
-        <v>2460</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="553" spans="1:3" x14ac:dyDescent="0.25">
@@ -14296,10 +14305,10 @@
         <v>1500</v>
       </c>
       <c r="B561" t="s">
-        <v>2461</v>
+        <v>2459</v>
       </c>
       <c r="C561" t="s">
-        <v>2462</v>
+        <v>2460</v>
       </c>
     </row>
     <row r="562" spans="1:3" x14ac:dyDescent="0.25">
@@ -14318,10 +14327,10 @@
         <v>1504</v>
       </c>
       <c r="B563" t="s">
-        <v>2463</v>
+        <v>2461</v>
       </c>
       <c r="C563" t="s">
-        <v>2464</v>
+        <v>2462</v>
       </c>
     </row>
     <row r="564" spans="1:3" x14ac:dyDescent="0.25">
@@ -14329,10 +14338,10 @@
         <v>1505</v>
       </c>
       <c r="B564" t="s">
-        <v>2465</v>
+        <v>2463</v>
       </c>
       <c r="C564" t="s">
-        <v>2466</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="565" spans="1:3" x14ac:dyDescent="0.25">
@@ -14351,10 +14360,10 @@
         <v>1509</v>
       </c>
       <c r="B566" t="s">
-        <v>2467</v>
+        <v>2465</v>
       </c>
       <c r="C566" t="s">
-        <v>2468</v>
+        <v>2466</v>
       </c>
     </row>
     <row r="567" spans="1:3" x14ac:dyDescent="0.25">
@@ -14373,10 +14382,10 @@
         <v>1513</v>
       </c>
       <c r="B568" t="s">
-        <v>2469</v>
+        <v>2467</v>
       </c>
       <c r="C568" t="s">
-        <v>2469</v>
+        <v>2467</v>
       </c>
     </row>
     <row r="569" spans="1:3" x14ac:dyDescent="0.25">
@@ -14395,10 +14404,10 @@
         <v>1517</v>
       </c>
       <c r="B570" t="s">
-        <v>2470</v>
+        <v>2468</v>
       </c>
       <c r="C570" t="s">
-        <v>2470</v>
+        <v>2468</v>
       </c>
     </row>
     <row r="571" spans="1:3" x14ac:dyDescent="0.25">
@@ -14417,10 +14426,10 @@
         <v>1521</v>
       </c>
       <c r="B572" t="s">
-        <v>2471</v>
+        <v>2469</v>
       </c>
       <c r="C572" t="s">
-        <v>2472</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="573" spans="1:3" x14ac:dyDescent="0.25">
@@ -14648,10 +14657,10 @@
         <v>1581</v>
       </c>
       <c r="B593" t="s">
-        <v>2473</v>
+        <v>2471</v>
       </c>
       <c r="C593" t="s">
-        <v>2474</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="594" spans="1:3" x14ac:dyDescent="0.25">
@@ -14703,10 +14712,10 @@
         <v>1594</v>
       </c>
       <c r="B598" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
       <c r="C598" t="s">
-        <v>2476</v>
+        <v>2474</v>
       </c>
     </row>
     <row r="599" spans="1:3" x14ac:dyDescent="0.25">
@@ -14846,10 +14855,10 @@
         <v>1630</v>
       </c>
       <c r="B611" t="s">
-        <v>2477</v>
+        <v>2475</v>
       </c>
       <c r="C611" t="s">
-        <v>2478</v>
+        <v>2476</v>
       </c>
     </row>
     <row r="612" spans="1:3" x14ac:dyDescent="0.25">
@@ -15253,10 +15262,10 @@
         <v>1736</v>
       </c>
       <c r="B648" t="s">
-        <v>2479</v>
+        <v>2477</v>
       </c>
       <c r="C648" t="s">
-        <v>2480</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="649" spans="1:3" x14ac:dyDescent="0.25">
@@ -15473,10 +15482,10 @@
         <v>1793</v>
       </c>
       <c r="B668" t="s">
-        <v>2481</v>
+        <v>2479</v>
       </c>
       <c r="C668" t="s">
-        <v>2482</v>
+        <v>2480</v>
       </c>
     </row>
     <row r="669" spans="1:3" x14ac:dyDescent="0.25">
@@ -15605,10 +15614,10 @@
         <v>1827</v>
       </c>
       <c r="B680" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
       <c r="C680" t="s">
-        <v>2484</v>
+        <v>2482</v>
       </c>
     </row>
     <row r="681" spans="1:3" x14ac:dyDescent="0.25">
@@ -15671,10 +15680,10 @@
         <v>1843</v>
       </c>
       <c r="B686" t="s">
-        <v>2485</v>
+        <v>2483</v>
       </c>
       <c r="C686" t="s">
-        <v>2485</v>
+        <v>2483</v>
       </c>
     </row>
     <row r="687" spans="1:3" x14ac:dyDescent="0.25">
@@ -15682,10 +15691,10 @@
         <v>1844</v>
       </c>
       <c r="B687" t="s">
-        <v>2486</v>
+        <v>2484</v>
       </c>
       <c r="C687" t="s">
-        <v>2487</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="688" spans="1:3" x14ac:dyDescent="0.25">
@@ -15693,10 +15702,10 @@
         <v>1845</v>
       </c>
       <c r="B688" t="s">
-        <v>2488</v>
+        <v>2486</v>
       </c>
       <c r="C688" t="s">
-        <v>2489</v>
+        <v>2487</v>
       </c>
     </row>
     <row r="689" spans="1:3" x14ac:dyDescent="0.25">
@@ -15759,10 +15768,10 @@
         <v>1861</v>
       </c>
       <c r="B694" t="s">
-        <v>2490</v>
+        <v>2488</v>
       </c>
       <c r="C694" t="s">
-        <v>2491</v>
+        <v>2489</v>
       </c>
     </row>
     <row r="695" spans="1:3" x14ac:dyDescent="0.25">
@@ -15781,10 +15790,10 @@
         <v>1865</v>
       </c>
       <c r="B696" t="s">
-        <v>2492</v>
+        <v>2490</v>
       </c>
       <c r="C696" t="s">
-        <v>2493</v>
+        <v>2491</v>
       </c>
     </row>
     <row r="697" spans="1:3" x14ac:dyDescent="0.25">
@@ -15924,10 +15933,10 @@
         <v>1902</v>
       </c>
       <c r="B709" t="s">
-        <v>2494</v>
+        <v>2492</v>
       </c>
       <c r="C709" t="s">
-        <v>2495</v>
+        <v>2493</v>
       </c>
     </row>
     <row r="710" spans="1:3" x14ac:dyDescent="0.25">
@@ -15935,10 +15944,10 @@
         <v>1903</v>
       </c>
       <c r="B710" t="s">
-        <v>2496</v>
+        <v>2494</v>
       </c>
       <c r="C710" t="s">
-        <v>2497</v>
+        <v>2495</v>
       </c>
     </row>
     <row r="711" spans="1:3" x14ac:dyDescent="0.25">
@@ -15946,10 +15955,10 @@
         <v>1904</v>
       </c>
       <c r="B711" t="s">
-        <v>2498</v>
+        <v>2496</v>
       </c>
       <c r="C711" t="s">
-        <v>2499</v>
+        <v>2497</v>
       </c>
     </row>
     <row r="712" spans="1:3" x14ac:dyDescent="0.25">
@@ -16001,10 +16010,10 @@
         <v>1917</v>
       </c>
       <c r="B716" t="s">
-        <v>2500</v>
+        <v>2498</v>
       </c>
       <c r="C716" t="s">
-        <v>2501</v>
+        <v>2499</v>
       </c>
     </row>
     <row r="717" spans="1:3" x14ac:dyDescent="0.25">
@@ -16427,1256 +16436,1267 @@
     </row>
     <row r="755" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
-        <v>2030</v>
+        <v>2555</v>
       </c>
       <c r="B755" t="s">
-        <v>2031</v>
+        <v>2556</v>
       </c>
       <c r="C755" t="s">
-        <v>2032</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="756" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
-        <v>2033</v>
+        <v>2030</v>
       </c>
       <c r="B756" t="s">
-        <v>2034</v>
+        <v>2031</v>
       </c>
       <c r="C756" t="s">
-        <v>2035</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="757" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>2036</v>
+        <v>2033</v>
       </c>
       <c r="B757" t="s">
-        <v>2037</v>
+        <v>2034</v>
       </c>
       <c r="C757" t="s">
-        <v>2038</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="758" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>2039</v>
+        <v>2036</v>
       </c>
       <c r="B758" t="s">
-        <v>2040</v>
+        <v>2037</v>
       </c>
       <c r="C758" t="s">
-        <v>2041</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="759" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>2042</v>
+        <v>2039</v>
       </c>
       <c r="B759" t="s">
-        <v>2043</v>
+        <v>2040</v>
       </c>
       <c r="C759" t="s">
-        <v>2044</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="760" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>2045</v>
+        <v>2042</v>
       </c>
       <c r="B760" t="s">
-        <v>2046</v>
+        <v>2043</v>
       </c>
       <c r="C760" t="s">
-        <v>2047</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="761" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
-        <v>2048</v>
+        <v>2045</v>
       </c>
       <c r="B761" t="s">
-        <v>2049</v>
+        <v>2046</v>
       </c>
       <c r="C761" t="s">
-        <v>2050</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="762" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A762" t="s">
-        <v>2051</v>
+        <v>2048</v>
       </c>
       <c r="B762" t="s">
-        <v>2052</v>
+        <v>2049</v>
       </c>
       <c r="C762" t="s">
-        <v>2053</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="763" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
       <c r="B763" t="s">
-        <v>2502</v>
+        <v>2052</v>
       </c>
       <c r="C763" t="s">
-        <v>2503</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="764" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A764" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="B764" t="s">
-        <v>2056</v>
+        <v>2500</v>
       </c>
       <c r="C764" t="s">
-        <v>2057</v>
+        <v>2501</v>
       </c>
     </row>
     <row r="765" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A765" t="s">
-        <v>2058</v>
+        <v>2055</v>
       </c>
       <c r="B765" t="s">
-        <v>2059</v>
+        <v>2056</v>
       </c>
       <c r="C765" t="s">
-        <v>2060</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="766" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
       <c r="B766" t="s">
-        <v>2062</v>
+        <v>2059</v>
       </c>
       <c r="C766" t="s">
-        <v>2063</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="767" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A767" t="s">
-        <v>2064</v>
+        <v>2061</v>
       </c>
       <c r="B767" t="s">
-        <v>2504</v>
+        <v>2062</v>
       </c>
       <c r="C767" t="s">
-        <v>2505</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="768" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A768" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="B768" t="s">
-        <v>2066</v>
+        <v>2502</v>
       </c>
       <c r="C768" t="s">
-        <v>2067</v>
+        <v>2503</v>
       </c>
     </row>
     <row r="769" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
-        <v>2068</v>
+        <v>2065</v>
       </c>
       <c r="B769" t="s">
-        <v>2069</v>
+        <v>2066</v>
       </c>
       <c r="C769" t="s">
-        <v>2070</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="770" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
-        <v>2071</v>
+        <v>2068</v>
       </c>
       <c r="B770" t="s">
-        <v>2072</v>
+        <v>2069</v>
       </c>
       <c r="C770" t="s">
-        <v>2073</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="771" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
-        <v>2074</v>
+        <v>2071</v>
       </c>
       <c r="B771" t="s">
-        <v>2506</v>
+        <v>2072</v>
       </c>
       <c r="C771" t="s">
-        <v>2507</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="772" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="B772" t="s">
-        <v>2508</v>
+        <v>2504</v>
       </c>
       <c r="C772" t="s">
-        <v>2509</v>
+        <v>2505</v>
       </c>
     </row>
     <row r="773" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="B773" t="s">
-        <v>2510</v>
+        <v>2506</v>
       </c>
       <c r="C773" t="s">
-        <v>2511</v>
+        <v>2507</v>
       </c>
     </row>
     <row r="774" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="B774" t="s">
-        <v>2078</v>
+        <v>2508</v>
       </c>
       <c r="C774" t="s">
-        <v>2079</v>
+        <v>2509</v>
       </c>
     </row>
     <row r="775" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
-        <v>2080</v>
+        <v>2077</v>
       </c>
       <c r="B775" t="s">
-        <v>2081</v>
+        <v>2078</v>
       </c>
       <c r="C775" t="s">
-        <v>2082</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="776" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
-        <v>2083</v>
+        <v>2080</v>
       </c>
       <c r="B776" t="s">
-        <v>2084</v>
+        <v>2081</v>
       </c>
       <c r="C776" t="s">
-        <v>2085</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="777" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
-        <v>2086</v>
+        <v>2083</v>
       </c>
       <c r="B777" t="s">
-        <v>2087</v>
+        <v>2084</v>
       </c>
       <c r="C777" t="s">
-        <v>2088</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="778" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
-        <v>2089</v>
+        <v>2086</v>
       </c>
       <c r="B778" t="s">
-        <v>2090</v>
+        <v>2087</v>
       </c>
       <c r="C778" t="s">
-        <v>2091</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="779" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
       <c r="B779" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="C779" t="s">
-        <v>2094</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="780" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
-        <v>2095</v>
+        <v>2092</v>
       </c>
       <c r="B780" t="s">
-        <v>2096</v>
+        <v>2093</v>
       </c>
       <c r="C780" t="s">
-        <v>2097</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="781" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>2098</v>
+        <v>2095</v>
       </c>
       <c r="B781" t="s">
-        <v>2099</v>
+        <v>2096</v>
       </c>
       <c r="C781" t="s">
-        <v>2100</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="782" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>2101</v>
+        <v>2098</v>
       </c>
       <c r="B782" t="s">
-        <v>2102</v>
+        <v>2099</v>
       </c>
       <c r="C782" t="s">
-        <v>2103</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="783" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
-        <v>2104</v>
+        <v>2101</v>
       </c>
       <c r="B783" t="s">
-        <v>2512</v>
+        <v>2102</v>
       </c>
       <c r="C783" t="s">
-        <v>2513</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="784" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="B784" t="s">
-        <v>2106</v>
+        <v>2510</v>
       </c>
       <c r="C784" t="s">
-        <v>2107</v>
+        <v>2511</v>
       </c>
     </row>
     <row r="785" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
-        <v>2108</v>
+        <v>2105</v>
       </c>
       <c r="B785" t="s">
-        <v>2109</v>
+        <v>2106</v>
       </c>
       <c r="C785" t="s">
-        <v>2110</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="786" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
-        <v>2111</v>
+        <v>2108</v>
       </c>
       <c r="B786" t="s">
-        <v>2514</v>
+        <v>2109</v>
       </c>
       <c r="C786" t="s">
-        <v>2515</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="787" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="B787" t="s">
-        <v>2516</v>
+        <v>2512</v>
       </c>
       <c r="C787" t="s">
-        <v>2517</v>
+        <v>2513</v>
       </c>
     </row>
     <row r="788" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="B788" t="s">
-        <v>2518</v>
+        <v>2514</v>
       </c>
       <c r="C788" t="s">
-        <v>2519</v>
+        <v>2515</v>
       </c>
     </row>
     <row r="789" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="B789" t="s">
-        <v>2115</v>
+        <v>2516</v>
       </c>
       <c r="C789" t="s">
-        <v>2116</v>
+        <v>2517</v>
       </c>
     </row>
     <row r="790" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>2117</v>
+        <v>2114</v>
       </c>
       <c r="B790" t="s">
-        <v>2118</v>
+        <v>2115</v>
       </c>
       <c r="C790" t="s">
-        <v>2119</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="791" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>2120</v>
+        <v>2117</v>
       </c>
       <c r="B791" t="s">
-        <v>2121</v>
+        <v>2118</v>
       </c>
       <c r="C791" t="s">
-        <v>2122</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="792" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>2123</v>
+        <v>2120</v>
       </c>
       <c r="B792" t="s">
-        <v>2124</v>
+        <v>2121</v>
       </c>
       <c r="C792" t="s">
-        <v>2125</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="793" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>2126</v>
+        <v>2123</v>
       </c>
       <c r="B793" t="s">
-        <v>2127</v>
+        <v>2124</v>
       </c>
       <c r="C793" t="s">
-        <v>2128</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="794" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>2129</v>
+        <v>2126</v>
       </c>
       <c r="B794" t="s">
-        <v>2130</v>
+        <v>2127</v>
       </c>
       <c r="C794" t="s">
-        <v>2131</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="795" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>2132</v>
+        <v>2129</v>
       </c>
       <c r="B795" t="s">
-        <v>2133</v>
+        <v>2130</v>
       </c>
       <c r="C795" t="s">
-        <v>2134</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="796" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>2135</v>
+        <v>2132</v>
       </c>
       <c r="B796" t="s">
-        <v>2136</v>
+        <v>2133</v>
       </c>
       <c r="C796" t="s">
-        <v>2137</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="797" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>2138</v>
+        <v>2135</v>
       </c>
       <c r="B797" t="s">
-        <v>2139</v>
+        <v>2136</v>
       </c>
       <c r="C797" t="s">
-        <v>2140</v>
+        <v>2137</v>
       </c>
     </row>
     <row r="798" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
-        <v>2141</v>
+        <v>2138</v>
       </c>
       <c r="B798" t="s">
-        <v>2142</v>
+        <v>2139</v>
       </c>
       <c r="C798" t="s">
-        <v>2143</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="799" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
-        <v>2144</v>
+        <v>2141</v>
       </c>
       <c r="B799" t="s">
-        <v>2145</v>
+        <v>2142</v>
       </c>
       <c r="C799" t="s">
-        <v>2146</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="800" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
-        <v>2147</v>
+        <v>2144</v>
       </c>
       <c r="B800" t="s">
-        <v>2520</v>
+        <v>2145</v>
       </c>
       <c r="C800" t="s">
-        <v>2521</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="801" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="B801" t="s">
-        <v>2149</v>
+        <v>2518</v>
       </c>
       <c r="C801" t="s">
-        <v>2150</v>
+        <v>2519</v>
       </c>
     </row>
     <row r="802" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
-        <v>2151</v>
+        <v>2148</v>
       </c>
       <c r="B802" t="s">
-        <v>2152</v>
+        <v>2149</v>
       </c>
       <c r="C802" t="s">
-        <v>2153</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="803" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
-        <v>2154</v>
+        <v>2151</v>
       </c>
       <c r="B803" t="s">
-        <v>2155</v>
+        <v>2152</v>
       </c>
       <c r="C803" t="s">
-        <v>2156</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="804" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A804" t="s">
-        <v>2157</v>
+        <v>2154</v>
       </c>
       <c r="B804" t="s">
-        <v>2158</v>
+        <v>2155</v>
       </c>
       <c r="C804" t="s">
-        <v>2159</v>
+        <v>2156</v>
       </c>
     </row>
     <row r="805" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
-        <v>2160</v>
+        <v>2157</v>
       </c>
       <c r="B805" t="s">
-        <v>2161</v>
+        <v>2158</v>
       </c>
       <c r="C805" t="s">
-        <v>2162</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="806" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
-        <v>2163</v>
+        <v>2160</v>
       </c>
       <c r="B806" t="s">
-        <v>2164</v>
+        <v>2161</v>
       </c>
       <c r="C806" t="s">
-        <v>2165</v>
+        <v>2162</v>
       </c>
     </row>
     <row r="807" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A807" t="s">
-        <v>2166</v>
+        <v>2163</v>
       </c>
       <c r="B807" t="s">
-        <v>2167</v>
+        <v>2164</v>
       </c>
       <c r="C807" t="s">
-        <v>1580</v>
+        <v>2165</v>
       </c>
     </row>
     <row r="808" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A808" t="s">
-        <v>2168</v>
+        <v>2166</v>
       </c>
       <c r="B808" t="s">
-        <v>2522</v>
+        <v>2167</v>
       </c>
       <c r="C808" t="s">
-        <v>2523</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="809" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A809" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="B809" t="s">
-        <v>2170</v>
+        <v>2520</v>
       </c>
       <c r="C809" t="s">
-        <v>2171</v>
+        <v>2521</v>
       </c>
     </row>
     <row r="810" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A810" t="s">
-        <v>2172</v>
+        <v>2169</v>
       </c>
       <c r="B810" t="s">
-        <v>2173</v>
+        <v>2170</v>
       </c>
       <c r="C810" t="s">
-        <v>2174</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="811" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A811" t="s">
-        <v>2175</v>
+        <v>2172</v>
       </c>
       <c r="B811" t="s">
-        <v>2176</v>
+        <v>2173</v>
       </c>
       <c r="C811" t="s">
-        <v>2177</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="812" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A812" t="s">
-        <v>2178</v>
+        <v>2175</v>
       </c>
       <c r="B812" t="s">
-        <v>2179</v>
+        <v>2176</v>
       </c>
       <c r="C812" t="s">
-        <v>2180</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="813" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
-        <v>2181</v>
+        <v>2178</v>
       </c>
       <c r="B813" t="s">
-        <v>3</v>
+        <v>2179</v>
       </c>
       <c r="C813" t="s">
-        <v>4</v>
+        <v>2180</v>
       </c>
     </row>
     <row r="814" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A814" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
       <c r="B814" t="s">
-        <v>2183</v>
+        <v>3</v>
       </c>
       <c r="C814" t="s">
-        <v>2184</v>
+        <v>4</v>
       </c>
     </row>
     <row r="815" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A815" t="s">
-        <v>2185</v>
+        <v>2182</v>
       </c>
       <c r="B815" t="s">
-        <v>2186</v>
+        <v>2183</v>
       </c>
       <c r="C815" t="s">
-        <v>2187</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="816" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A816" t="s">
-        <v>2188</v>
+        <v>2185</v>
       </c>
       <c r="B816" t="s">
-        <v>2189</v>
+        <v>2186</v>
       </c>
       <c r="C816" t="s">
-        <v>2190</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="817" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A817" t="s">
-        <v>2191</v>
+        <v>2188</v>
       </c>
       <c r="B817" t="s">
-        <v>2192</v>
+        <v>2189</v>
       </c>
       <c r="C817" t="s">
-        <v>2193</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="818" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A818" t="s">
-        <v>2194</v>
+        <v>2191</v>
       </c>
       <c r="B818" t="s">
-        <v>2195</v>
+        <v>2192</v>
       </c>
       <c r="C818" t="s">
-        <v>2196</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="819" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A819" t="s">
-        <v>2197</v>
+        <v>2194</v>
       </c>
       <c r="B819" t="s">
-        <v>2198</v>
+        <v>2195</v>
       </c>
       <c r="C819" t="s">
-        <v>2199</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="820" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A820" t="s">
-        <v>2200</v>
+        <v>2197</v>
       </c>
       <c r="B820" t="s">
-        <v>2201</v>
+        <v>2198</v>
       </c>
       <c r="C820" t="s">
-        <v>378</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="821" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A821" t="s">
-        <v>2202</v>
+        <v>2200</v>
       </c>
       <c r="B821" t="s">
-        <v>2203</v>
+        <v>2201</v>
       </c>
       <c r="C821" t="s">
-        <v>2204</v>
+        <v>378</v>
       </c>
     </row>
     <row r="822" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A822" t="s">
-        <v>2205</v>
+        <v>2202</v>
       </c>
       <c r="B822" t="s">
-        <v>2206</v>
+        <v>2203</v>
       </c>
       <c r="C822" t="s">
-        <v>2207</v>
+        <v>2204</v>
       </c>
     </row>
     <row r="823" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A823" t="s">
-        <v>2208</v>
+        <v>2205</v>
       </c>
       <c r="B823" t="s">
-        <v>191</v>
+        <v>2206</v>
       </c>
       <c r="C823" t="s">
-        <v>192</v>
+        <v>2207</v>
       </c>
     </row>
     <row r="824" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A824" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
       <c r="B824" t="s">
-        <v>2210</v>
+        <v>191</v>
       </c>
       <c r="C824" t="s">
-        <v>2211</v>
+        <v>192</v>
       </c>
     </row>
     <row r="825" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A825" t="s">
-        <v>2212</v>
+        <v>2209</v>
       </c>
       <c r="B825" t="s">
-        <v>2213</v>
+        <v>2210</v>
       </c>
       <c r="C825" t="s">
-        <v>2214</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="826" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A826" t="s">
-        <v>2215</v>
+        <v>2212</v>
       </c>
       <c r="B826" t="s">
-        <v>2216</v>
+        <v>2213</v>
       </c>
       <c r="C826" t="s">
-        <v>2217</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="827" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A827" t="s">
-        <v>2218</v>
+        <v>2215</v>
       </c>
       <c r="B827" t="s">
-        <v>2219</v>
+        <v>2216</v>
       </c>
       <c r="C827" t="s">
-        <v>2220</v>
+        <v>2217</v>
       </c>
     </row>
     <row r="828" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A828" t="s">
-        <v>2221</v>
+        <v>2218</v>
       </c>
       <c r="B828" t="s">
-        <v>2222</v>
+        <v>2219</v>
       </c>
       <c r="C828" t="s">
-        <v>2223</v>
+        <v>2220</v>
       </c>
     </row>
     <row r="829" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A829" t="s">
-        <v>2224</v>
+        <v>2221</v>
       </c>
       <c r="B829" t="s">
-        <v>2225</v>
+        <v>2222</v>
       </c>
       <c r="C829" t="s">
-        <v>2226</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="830" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A830" t="s">
-        <v>2227</v>
+        <v>2224</v>
       </c>
       <c r="B830" t="s">
-        <v>2228</v>
+        <v>2225</v>
       </c>
       <c r="C830" t="s">
-        <v>2229</v>
+        <v>2226</v>
       </c>
     </row>
     <row r="831" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A831" t="s">
-        <v>2230</v>
+        <v>2227</v>
       </c>
       <c r="B831" t="s">
-        <v>2231</v>
+        <v>2228</v>
       </c>
       <c r="C831" t="s">
-        <v>2232</v>
+        <v>2229</v>
       </c>
     </row>
     <row r="832" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A832" t="s">
-        <v>2233</v>
+        <v>2230</v>
       </c>
       <c r="B832" t="s">
-        <v>2234</v>
+        <v>2231</v>
       </c>
       <c r="C832" t="s">
-        <v>2235</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="833" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A833" t="s">
-        <v>2236</v>
+        <v>2233</v>
       </c>
       <c r="B833" t="s">
-        <v>2237</v>
+        <v>2553</v>
       </c>
       <c r="C833" t="s">
-        <v>2238</v>
+        <v>2554</v>
       </c>
     </row>
     <row r="834" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A834" t="s">
-        <v>2239</v>
+        <v>2234</v>
       </c>
       <c r="B834" t="s">
-        <v>2240</v>
+        <v>2235</v>
       </c>
       <c r="C834" t="s">
-        <v>2241</v>
+        <v>2236</v>
       </c>
     </row>
     <row r="835" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
-        <v>2242</v>
+        <v>2237</v>
       </c>
       <c r="B835" t="s">
-        <v>2243</v>
+        <v>2238</v>
       </c>
       <c r="C835" t="s">
-        <v>2243</v>
+        <v>2239</v>
       </c>
     </row>
     <row r="836" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A836" t="s">
-        <v>2244</v>
+        <v>2240</v>
       </c>
       <c r="B836" t="s">
-        <v>2245</v>
+        <v>2241</v>
       </c>
       <c r="C836" t="s">
-        <v>2246</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="837" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A837" t="s">
-        <v>2247</v>
+        <v>2242</v>
       </c>
       <c r="B837" t="s">
-        <v>2248</v>
+        <v>2243</v>
       </c>
       <c r="C837" t="s">
-        <v>2214</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="838" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
-        <v>2249</v>
+        <v>2245</v>
       </c>
       <c r="B838" t="s">
-        <v>2250</v>
+        <v>2246</v>
       </c>
       <c r="C838" t="s">
-        <v>2251</v>
+        <v>2214</v>
       </c>
     </row>
     <row r="839" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A839" t="s">
-        <v>2252</v>
+        <v>2247</v>
       </c>
       <c r="B839" t="s">
-        <v>2253</v>
+        <v>2248</v>
       </c>
       <c r="C839" t="s">
-        <v>2254</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="840" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A840" t="s">
-        <v>2255</v>
+        <v>2250</v>
       </c>
       <c r="B840" t="s">
-        <v>2256</v>
+        <v>2251</v>
       </c>
       <c r="C840" t="s">
-        <v>2257</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="841" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
-        <v>2258</v>
+        <v>2253</v>
       </c>
       <c r="B841" t="s">
-        <v>2259</v>
+        <v>2254</v>
       </c>
       <c r="C841" t="s">
-        <v>2260</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="842" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
-        <v>2261</v>
+        <v>2256</v>
       </c>
       <c r="B842" t="s">
-        <v>2262</v>
+        <v>2257</v>
       </c>
       <c r="C842" t="s">
-        <v>2263</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="843" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A843" t="s">
-        <v>2264</v>
+        <v>2259</v>
       </c>
       <c r="B843" t="s">
-        <v>2265</v>
+        <v>2260</v>
       </c>
       <c r="C843" t="s">
-        <v>2266</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="844" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A844" t="s">
-        <v>2267</v>
+        <v>2262</v>
       </c>
       <c r="B844" t="s">
-        <v>2268</v>
+        <v>2263</v>
       </c>
       <c r="C844" t="s">
-        <v>2269</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="845" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A845" t="s">
-        <v>2270</v>
+        <v>2265</v>
       </c>
       <c r="B845" t="s">
-        <v>2271</v>
+        <v>2266</v>
       </c>
       <c r="C845" t="s">
-        <v>2272</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="846" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A846" t="s">
-        <v>2273</v>
+        <v>2268</v>
       </c>
       <c r="B846" t="s">
-        <v>2274</v>
+        <v>2269</v>
       </c>
       <c r="C846" t="s">
-        <v>2275</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="847" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A847" t="s">
-        <v>2276</v>
+        <v>2271</v>
       </c>
       <c r="B847" t="s">
-        <v>2277</v>
+        <v>2272</v>
       </c>
       <c r="C847" t="s">
-        <v>2278</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="848" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A848" t="s">
-        <v>2279</v>
+        <v>2274</v>
       </c>
       <c r="B848" t="s">
-        <v>2280</v>
+        <v>2275</v>
       </c>
       <c r="C848" t="s">
-        <v>2281</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="849" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A849" t="s">
-        <v>2282</v>
+        <v>2277</v>
       </c>
       <c r="B849" t="s">
-        <v>2283</v>
+        <v>2278</v>
       </c>
       <c r="C849" t="s">
-        <v>2284</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="850" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A850" t="s">
-        <v>2285</v>
+        <v>2280</v>
       </c>
       <c r="B850" t="s">
-        <v>2286</v>
+        <v>2281</v>
       </c>
       <c r="C850" t="s">
-        <v>2287</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="851" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
-        <v>2288</v>
+        <v>2283</v>
       </c>
       <c r="B851" t="s">
-        <v>2289</v>
+        <v>2284</v>
       </c>
       <c r="C851" t="s">
-        <v>2290</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="852" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A852" t="s">
-        <v>2291</v>
+        <v>2286</v>
       </c>
       <c r="B852" t="s">
-        <v>2292</v>
+        <v>2287</v>
       </c>
       <c r="C852" t="s">
-        <v>950</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="853" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A853" t="s">
-        <v>2293</v>
+        <v>2289</v>
       </c>
       <c r="B853" t="s">
-        <v>2294</v>
+        <v>2290</v>
       </c>
       <c r="C853" t="s">
-        <v>2295</v>
+        <v>950</v>
       </c>
     </row>
     <row r="854" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A854" t="s">
-        <v>2296</v>
+        <v>2291</v>
       </c>
       <c r="B854" t="s">
-        <v>2297</v>
+        <v>2292</v>
       </c>
       <c r="C854" t="s">
-        <v>2298</v>
+        <v>2293</v>
       </c>
     </row>
     <row r="855" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A855" t="s">
-        <v>2299</v>
+        <v>2294</v>
       </c>
       <c r="B855" t="s">
-        <v>2300</v>
+        <v>2295</v>
       </c>
       <c r="C855" t="s">
-        <v>2301</v>
+        <v>2296</v>
       </c>
     </row>
     <row r="856" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A856" t="s">
-        <v>2302</v>
+        <v>2297</v>
       </c>
       <c r="B856" t="s">
-        <v>2303</v>
+        <v>2298</v>
       </c>
       <c r="C856" t="s">
-        <v>2304</v>
+        <v>2299</v>
       </c>
     </row>
     <row r="857" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A857" t="s">
-        <v>2305</v>
+        <v>2300</v>
       </c>
       <c r="B857" t="s">
-        <v>2306</v>
+        <v>2301</v>
       </c>
       <c r="C857" t="s">
-        <v>2307</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="858" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A858" t="s">
-        <v>2308</v>
+        <v>2303</v>
       </c>
       <c r="B858" t="s">
-        <v>2524</v>
+        <v>2304</v>
       </c>
       <c r="C858" t="s">
-        <v>2525</v>
-      </c>
-    </row>
-    <row r="860" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A860" t="s">
-        <v>2526</v>
-      </c>
-      <c r="B860" t="s">
-        <v>2529</v>
-      </c>
-      <c r="C860" t="s">
-        <v>2535</v>
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="859" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A859" t="s">
+        <v>2306</v>
+      </c>
+      <c r="B859" t="s">
+        <v>2522</v>
+      </c>
+      <c r="C859" t="s">
+        <v>2523</v>
       </c>
     </row>
     <row r="861" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A861" t="s">
+        <v>2524</v>
+      </c>
+      <c r="B861" t="s">
         <v>2527</v>
       </c>
-      <c r="B861" t="s">
-        <v>2530</v>
-      </c>
       <c r="C861" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
     </row>
     <row r="862" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A862" t="s">
+        <v>2525</v>
+      </c>
+      <c r="B862" t="s">
         <v>2528</v>
       </c>
-      <c r="B862" t="s">
-        <v>2531</v>
-      </c>
       <c r="C862" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
     </row>
     <row r="863" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A863" t="s">
-        <v>2532</v>
+        <v>2526</v>
       </c>
       <c r="B863" t="s">
-        <v>2536</v>
+        <v>2529</v>
       </c>
       <c r="C863" t="s">
-        <v>2537</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="864" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A864" t="s">
-        <v>2538</v>
+        <v>2530</v>
       </c>
       <c r="B864" t="s">
-        <v>2539</v>
+        <v>2534</v>
       </c>
       <c r="C864" t="s">
-        <v>2540</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="865" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
-        <v>2541</v>
+        <v>2536</v>
       </c>
       <c r="B865" t="s">
-        <v>2542</v>
+        <v>2537</v>
       </c>
       <c r="C865" t="s">
-        <v>2543</v>
+        <v>2538</v>
       </c>
     </row>
     <row r="866" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
-        <v>2545</v>
-      </c>
-      <c r="B866" s="1" t="s">
-        <v>2546</v>
+        <v>2539</v>
+      </c>
+      <c r="B866" t="s">
+        <v>2540</v>
       </c>
       <c r="C866" t="s">
-        <v>2548</v>
+        <v>2541</v>
       </c>
     </row>
     <row r="867" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
+        <v>2543</v>
+      </c>
+      <c r="B867" s="1" t="s">
         <v>2544</v>
       </c>
-      <c r="B867" s="1" t="s">
-        <v>2547</v>
-      </c>
       <c r="C867" t="s">
-        <v>2549</v>
+        <v>2546</v>
       </c>
     </row>
     <row r="868" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A868" t="s">
+        <v>2542</v>
+      </c>
+      <c r="B868" s="1" t="s">
+        <v>2545</v>
+      </c>
+      <c r="C868" t="s">
+        <v>2547</v>
+      </c>
+    </row>
+    <row r="869" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A869" t="s">
+        <v>2548</v>
+      </c>
+      <c r="B869" t="s">
+        <v>2549</v>
+      </c>
+      <c r="C869" t="s">
         <v>2550</v>
       </c>
-      <c r="B868" t="s">
+    </row>
+    <row r="870" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A870" s="1" t="s">
         <v>2551</v>
       </c>
-      <c r="C868" t="s">
+      <c r="B870" t="s">
+        <v>227</v>
+      </c>
+      <c r="C870" t="s">
         <v>2552</v>
-      </c>
-    </row>
-    <row r="869" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A869" s="1" t="s">
-        <v>2553</v>
-      </c>
-      <c r="B869" t="s">
-        <v>227</v>
-      </c>
-      <c r="C869" t="s">
-        <v>2554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all checks on server, new string constants for web client
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56038583-6252-433F-BA01-41832CEC87BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AF5888-962F-42BB-B007-FD11229348E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="600" windowWidth="26250" windowHeight="13545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2100" yWindow="750" windowWidth="26250" windowHeight="13545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2688" uniqueCount="2636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="2639">
   <si>
     <t>Name</t>
   </si>
@@ -7932,6 +7932,15 @@
   </si>
   <si>
     <t>{{0}}:  Настройки мониторинга</t>
+  </si>
+  <si>
+    <t>SID_Landmark_count_does_not_match_graph</t>
+  </si>
+  <si>
+    <t>Количество ориентиров на рефлектограмме не соответствует графу</t>
+  </si>
+  <si>
+    <t>Landmark count on base ref does not match graph</t>
   </si>
 </sst>
 </file>
@@ -7979,13 +7988,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8329,10 +8339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C897"/>
+  <dimension ref="A1:C898"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A881" workbookViewId="0">
-      <selection activeCell="B901" sqref="B901"/>
+    <sheetView tabSelected="1" topLeftCell="A876" workbookViewId="0">
+      <selection activeCell="A898" sqref="A898"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18198,6 +18208,17 @@
         <v>2633</v>
       </c>
     </row>
+    <row r="898" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A898" s="4" t="s">
+        <v>2636</v>
+      </c>
+      <c r="B898" s="4" t="s">
+        <v>2638</v>
+      </c>
+      <c r="C898" s="4" t="s">
+        <v>2637</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
attach otau component localization
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AECC97-52A7-46B2-949A-754AFAD6A18F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E10D062-479F-4BE8-B392-6C7E6193C2B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2691" uniqueCount="2639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2697" uniqueCount="2644">
   <si>
     <t>Name</t>
   </si>
@@ -7941,13 +7941,28 @@
   </si>
   <si>
     <t>State at {{0}} (ID {{1}})</t>
+  </si>
+  <si>
+    <t>Attach optical switch</t>
+  </si>
+  <si>
+    <t>Optical switch's IP address</t>
+  </si>
+  <si>
+    <t>SID_Optical_switch_s_IP_address</t>
+  </si>
+  <si>
+    <t>Подключить оптический переключатель</t>
+  </si>
+  <si>
+    <t>IP адрес оптического переключателя</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -7964,6 +7979,12 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="204"/>
     </font>
   </fonts>
@@ -7988,7 +8009,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -7996,6 +8017,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8339,10 +8364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C898"/>
+  <dimension ref="A1:C900"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A400" workbookViewId="0">
-      <selection activeCell="A419" sqref="A419"/>
+    <sheetView tabSelected="1" topLeftCell="A874" workbookViewId="0">
+      <selection activeCell="C901" sqref="C901"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18219,7 +18244,30 @@
         <v>2635</v>
       </c>
     </row>
+    <row r="899" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A899" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="B899" s="5" t="s">
+        <v>2639</v>
+      </c>
+      <c r="C899" s="6" t="s">
+        <v>2642</v>
+      </c>
+    </row>
+    <row r="900" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A900" s="5" t="s">
+        <v>2641</v>
+      </c>
+      <c r="B900" s="5" t="s">
+        <v>2640</v>
+      </c>
+      <c r="C900" s="6" t="s">
+        <v>2643</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
some string constants, offset between ref and base
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E492B819-230E-428F-95CC-E605FE9A6EC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D03FEB-8069-4E80-A824-59BC77AA6BF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24495" yWindow="1830" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2703" uniqueCount="2650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2709" uniqueCount="2656">
   <si>
     <t>Name</t>
   </si>
@@ -7974,6 +7974,24 @@
   </si>
   <si>
     <t>Верия ПО Web API</t>
+  </si>
+  <si>
+    <t>SID_Save_reflectogram</t>
+  </si>
+  <si>
+    <t>SID_Save_ref_and_base</t>
+  </si>
+  <si>
+    <t>Save reflectogram</t>
+  </si>
+  <si>
+    <t>Save ref + base</t>
+  </si>
+  <si>
+    <t>Сохранить рефлектограмму</t>
+  </si>
+  <si>
+    <t>Сохранить рефлектограмму + базовую</t>
   </si>
 </sst>
 </file>
@@ -8391,10 +8409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C902"/>
+  <dimension ref="A1:C904"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView tabSelected="1" topLeftCell="A885" workbookViewId="0">
+      <selection activeCell="C905" sqref="C905"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18315,6 +18333,28 @@
         <v>2649</v>
       </c>
     </row>
+    <row r="903" spans="1:3">
+      <c r="A903" t="s">
+        <v>2650</v>
+      </c>
+      <c r="B903" t="s">
+        <v>2652</v>
+      </c>
+      <c r="C903" t="s">
+        <v>2654</v>
+      </c>
+    </row>
+    <row r="904" spans="1:3">
+      <c r="A904" t="s">
+        <v>2651</v>
+      </c>
+      <c r="B904" t="s">
+        <v>2653</v>
+      </c>
+      <c r="C904" t="s">
+        <v>2655</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
rfts events - first approximation
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8688F86-2E27-46A2-ADEC-ADA97E78A656}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560328CB-1D44-401F-81A8-9C4F88D5BE30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24435" yWindow="1980" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1590" yWindow="1140" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2709" uniqueCount="2656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="2662">
   <si>
     <t>Name</t>
   </si>
@@ -7992,6 +7992,24 @@
   </si>
   <si>
     <t>Log in</t>
+  </si>
+  <si>
+    <t>SID_Logout</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>RTUs</t>
+  </si>
+  <si>
+    <t>Выйти</t>
+  </si>
+  <si>
+    <t>Модули</t>
+  </si>
+  <si>
+    <t>SID_RTU_Tree</t>
   </si>
 </sst>
 </file>
@@ -8409,10 +8427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C904"/>
+  <dimension ref="A1:C906"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView tabSelected="1" topLeftCell="A892" workbookViewId="0">
+      <selection activeCell="A910" sqref="A910"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18355,6 +18373,28 @@
         <v>2654</v>
       </c>
     </row>
+    <row r="905" spans="1:3">
+      <c r="A905" t="s">
+        <v>2656</v>
+      </c>
+      <c r="B905" t="s">
+        <v>2657</v>
+      </c>
+      <c r="C905" t="s">
+        <v>2659</v>
+      </c>
+    </row>
+    <row r="906" spans="1:3">
+      <c r="A906" t="s">
+        <v>2661</v>
+      </c>
+      <c r="B906" t="s">
+        <v>2658</v>
+      </c>
+      <c r="C906" t="s">
+        <v>2660</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
optical, network and bop event tables are colored
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9781E901-C57E-4853-83A3-C5C0DCC37841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33BE41B-11C5-4A18-B8ED-EE4C770D1A51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="1245" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4710" yWindow="1035" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="1" r:id="rId1"/>
@@ -8429,8 +8429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C906"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A373" workbookViewId="0">
-      <selection activeCell="A385" sqref="A385"/>
+    <sheetView tabSelected="1" topLeftCell="A412" workbookViewId="0">
+      <selection activeCell="A424" sqref="A424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Prohibit set automatic monitoring mode if no traces selected
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33BE41B-11C5-4A18-B8ED-EE4C770D1A51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50000E41-9EAB-4250-B0F2-7C9D8BCB56A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="1035" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="2662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2724" uniqueCount="2669">
   <si>
     <t>Name</t>
   </si>
@@ -8010,6 +8010,27 @@
   </si>
   <si>
     <t>SID_RTU_Tree</t>
+  </si>
+  <si>
+    <t>SID_Reject</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>Отклонить</t>
+  </si>
+  <si>
+    <t>SID_Yes</t>
+  </si>
+  <si>
+    <t>SID_No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Да</t>
   </si>
 </sst>
 </file>
@@ -8427,10 +8448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C906"/>
+  <dimension ref="A1:C909"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A412" workbookViewId="0">
-      <selection activeCell="A424" sqref="A424"/>
+    <sheetView tabSelected="1" topLeftCell="B904" workbookViewId="0">
+      <selection activeCell="C910" sqref="C910"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18395,6 +18416,39 @@
         <v>2660</v>
       </c>
     </row>
+    <row r="907" spans="1:3">
+      <c r="A907" t="s">
+        <v>2662</v>
+      </c>
+      <c r="B907" t="s">
+        <v>2663</v>
+      </c>
+      <c r="C907" t="s">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="908" spans="1:3">
+      <c r="A908" t="s">
+        <v>2665</v>
+      </c>
+      <c r="B908" t="s">
+        <v>2667</v>
+      </c>
+      <c r="C908" t="s">
+        <v>2668</v>
+      </c>
+    </row>
+    <row r="909" spans="1:3">
+      <c r="A909" t="s">
+        <v>2666</v>
+      </c>
+      <c r="B909" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C909" t="s">
+        <v>1133</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
some log points added
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4088ED2-F813-4537-90F5-DC2F5CF24705}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC8E094-EE98-484D-B1EC-F427FE8B4645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4290" yWindow="1365" windowWidth="22275" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8213,13 +8213,13 @@
     <t>О системе</t>
   </si>
   <si>
-    <t>Application closed</t>
-  </si>
-  <si>
-    <t>Приложение закрыто</t>
-  </si>
-  <si>
     <t>SID_Application_closed</t>
+  </si>
+  <si>
+    <t>Application closed.</t>
+  </si>
+  <si>
+    <t>Приложение закрыто.</t>
   </si>
 </sst>
 </file>
@@ -8648,7 +8648,7 @@
   <dimension ref="A1:C930"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A913" workbookViewId="0">
-      <selection activeCell="A932" sqref="A932"/>
+      <selection activeCell="B932" sqref="B932"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18868,13 +18868,13 @@
     </row>
     <row r="930" spans="1:3">
       <c r="A930" t="s">
+        <v>2729</v>
+      </c>
+      <c r="B930" t="s">
+        <v>2730</v>
+      </c>
+      <c r="C930" t="s">
         <v>2731</v>
-      </c>
-      <c r="B930" t="s">
-        <v>2729</v>
-      </c>
-      <c r="C930" t="s">
-        <v>2730</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
compare web client's and web API's versions
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC8E094-EE98-484D-B1EC-F427FE8B4645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF070BE-561D-42CF-A6A0-416D865B8008}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="1365" windowWidth="22275" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23895" yWindow="1470" windowWidth="22275" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2787" uniqueCount="2732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2793" uniqueCount="2738">
   <si>
     <t>Name</t>
   </si>
@@ -8220,6 +8220,24 @@
   </si>
   <si>
     <t>Приложение закрыто.</t>
+  </si>
+  <si>
+    <t>SID_Versions_do_not_match</t>
+  </si>
+  <si>
+    <t>Client's version does not match server's one!</t>
+  </si>
+  <si>
+    <t>Версия клиента не совпадает с версией сервера</t>
+  </si>
+  <si>
+    <t>SID_Please_close_browser</t>
+  </si>
+  <si>
+    <t>Please close browser's tab and start Fibertest again.</t>
+  </si>
+  <si>
+    <t>Пожалуйста, закройте вкладку браузера и запустите Fibertest снова.</t>
   </si>
 </sst>
 </file>
@@ -8645,10 +8663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C930"/>
+  <dimension ref="A1:C932"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A913" workbookViewId="0">
-      <selection activeCell="B932" sqref="B932"/>
+      <selection activeCell="C933" sqref="C933"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18877,6 +18895,28 @@
         <v>2731</v>
       </c>
     </row>
+    <row r="931" spans="1:3">
+      <c r="A931" t="s">
+        <v>2732</v>
+      </c>
+      <c r="B931" t="s">
+        <v>2733</v>
+      </c>
+      <c r="C931" t="s">
+        <v>2734</v>
+      </c>
+    </row>
+    <row r="932" spans="1:3">
+      <c r="A932" t="s">
+        <v>2735</v>
+      </c>
+      <c r="B932" s="5" t="s">
+        <v>2736</v>
+      </c>
+      <c r="C932" s="5" t="s">
+        <v>2737</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
sor viewer opens with closed settings panel
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF070BE-561D-42CF-A6A0-416D865B8008}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676919A4-EBD0-4A74-A8EB-CFFFB54951A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23895" yWindow="1470" windowWidth="22275" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="1500" windowWidth="22275" windowHeight="12615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="1" r:id="rId1"/>
@@ -8237,7 +8237,7 @@
     <t>Please close browser's tab and start Fibertest again.</t>
   </si>
   <si>
-    <t>Пожалуйста, закройте вкладку браузера и запустите Fibertest снова.</t>
+    <t>Пожалуйста, закройте вкладку браузера и повторите подключение в новой вкладке.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
web client free port gets correct otauId, web client trace attach to bop gets correct otauId so attach trace and measurement Client work correctly
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest20\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A130B6DD-DC14-4E7A-B363-C770084F146B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8966D19A-DC59-4432-AC97-DBDFBEE136C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1605" windowWidth="25305" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="1" r:id="rId1"/>
@@ -9973,16 +9973,16 @@
     <t>RTU {{0}} занят.</t>
   </si>
   <si>
-    <t xml:space="preserve">{{{{{{{{0}}}}}}}}: Monitoring Settings </t>
-  </si>
-  <si>
-    <t>{{{{{{{{0}}}}}}}}:  Настройки мониторинга</t>
-  </si>
-  <si>
-    <t>Cycle full time {{{{{{{{0}}}}}}}} sec</t>
-  </si>
-  <si>
-    <t>Полное время цикла {{{{{{{{0}}}}}}}} сек</t>
+    <t xml:space="preserve">{{0}}: Monitoring Settings </t>
+  </si>
+  <si>
+    <t>Cycle full time {{0}} sec</t>
+  </si>
+  <si>
+    <t>{{0}}:  Настройки мониторинга</t>
+  </si>
+  <si>
+    <t>Полное время цикла {{0}} сек</t>
   </si>
 </sst>
 </file>
@@ -10407,8 +10407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A415" sqref="A415"/>
+    <sheetView tabSelected="1" topLeftCell="A1103" workbookViewId="0">
+      <selection activeCell="C1105" sqref="C1105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20230,7 +20230,7 @@
         <v>2407</v>
       </c>
     </row>
-    <row r="893" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
         <v>2408</v>
       </c>
@@ -22516,7 +22516,7 @@
         <v>3313</v>
       </c>
       <c r="C1101" s="2" t="s">
-        <v>3314</v>
+        <v>3315</v>
       </c>
     </row>
     <row r="1102" spans="1:3" x14ac:dyDescent="0.25">
@@ -22546,7 +22546,7 @@
         <v>3002</v>
       </c>
       <c r="B1104" s="2" t="s">
-        <v>3315</v>
+        <v>3314</v>
       </c>
       <c r="C1104" s="2" t="s">
         <v>3316</v>

</xml_diff>

<commit_message>
Landmarks table renewed in Web Client
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest20\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8966D19A-DC59-4432-AC97-DBDFBEE136C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5116FF44-E638-4A13-B0EE-359EFF7F3BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="780" windowWidth="23430" windowHeight="13455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fibertest" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3360" uniqueCount="3317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3423" uniqueCount="3379">
   <si>
     <t>Name</t>
   </si>
@@ -4295,7 +4295,7 @@
     <t>Equipment title</t>
   </si>
   <si>
-    <t>Название оборуд.</t>
+    <t>Название оборудования</t>
   </si>
   <si>
     <t>SID_Go_to_the_fork</t>
@@ -8966,223 +8966,181 @@
     <t>Применяются настройки мониторинга</t>
   </si>
   <si>
-    <t>en-US</t>
-  </si>
-  <si>
-    <t>ru-RU</t>
-  </si>
-  <si>
-    <t>SID_Items_per_page</t>
-  </si>
-  <si>
-    <t>Items per page</t>
-  </si>
-  <si>
-    <t>Строк на странице</t>
-  </si>
-  <si>
-    <t>SID_Next_page</t>
-  </si>
-  <si>
-    <t>Next page</t>
-  </si>
-  <si>
-    <t>Следующая страница</t>
-  </si>
-  <si>
-    <t>SID_Previous_page</t>
-  </si>
-  <si>
-    <t>Previous page</t>
-  </si>
-  <si>
-    <t>Предыдущая страница</t>
-  </si>
-  <si>
-    <t>SID_of</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> of </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> из </t>
-  </si>
-  <si>
-    <t>SID_Responsive</t>
-  </si>
-  <si>
-    <t>Responsive</t>
-  </si>
-  <si>
-    <t>Отзывчивый</t>
-  </si>
-  <si>
-    <t>SID_Rtu_Moni_Settings</t>
-  </si>
-  <si>
-    <t>SID_measurement_frequency</t>
-  </si>
-  <si>
-    <t>measurement frequency</t>
-  </si>
-  <si>
-    <t>частота измерений</t>
-  </si>
-  <si>
-    <t>SID_saving_frequency</t>
-  </si>
-  <si>
-    <t>saving frequency</t>
-  </si>
-  <si>
-    <t>частота сохранения</t>
-  </si>
-  <si>
-    <t>SID_Cycle_full_time_sec</t>
-  </si>
-  <si>
-    <t>SID_Auto</t>
-  </si>
-  <si>
-    <t>Авто</t>
-  </si>
-  <si>
-    <t>SID_Landmark_count_does_not_match_graph</t>
-  </si>
-  <si>
-    <t>Landmark count on base ref does not match graph</t>
-  </si>
-  <si>
-    <t>Количество ориентиров на рефлектограмме не соответствует графу</t>
-  </si>
-  <si>
-    <t>Attach optical switch</t>
-  </si>
-  <si>
-    <t>Подключить оптический переключатель</t>
-  </si>
-  <si>
-    <t>SID_Optical_switch_s_IP_address</t>
-  </si>
-  <si>
-    <t>Optical switch's IP address</t>
-  </si>
-  <si>
-    <t>IP адрес оптического переключателя</t>
-  </si>
-  <si>
-    <t>SID_Web_Client_software_version</t>
-  </si>
-  <si>
-    <t>Web-Client software version</t>
-  </si>
-  <si>
-    <t>Версия ПК WebClient</t>
-  </si>
-  <si>
-    <t>SID_Web_Api_software_version</t>
-  </si>
-  <si>
-    <t>Web API software version</t>
-  </si>
-  <si>
-    <t>Верия ПК Web API</t>
-  </si>
-  <si>
-    <t>SID_Save_reflectogram</t>
-  </si>
-  <si>
-    <t>Save reflectogram</t>
-  </si>
-  <si>
-    <t>Сохранить рефлектограмму</t>
-  </si>
-  <si>
-    <t>SID_Save_ref_and_base</t>
-  </si>
-  <si>
-    <t>Save ref + base</t>
-  </si>
-  <si>
-    <t>Сохранить рефлектограмму + базовую</t>
-  </si>
-  <si>
-    <t>SID_Logout</t>
-  </si>
-  <si>
-    <t>Logout</t>
-  </si>
-  <si>
-    <t>Выйти</t>
-  </si>
-  <si>
-    <t>SID_RTU_Tree</t>
-  </si>
-  <si>
-    <t>RTUs</t>
-  </si>
-  <si>
-    <t>Модули</t>
-  </si>
-  <si>
-    <t>SID_Reject</t>
-  </si>
-  <si>
-    <t>Reject</t>
-  </si>
-  <si>
-    <t>Отклонить</t>
-  </si>
-  <si>
-    <t>SID_Yes</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Да</t>
-  </si>
-  <si>
-    <t>SID_No</t>
-  </si>
-  <si>
-    <t>SID_Device</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>Устройство</t>
-  </si>
-  <si>
-    <t>SID_Application_closed</t>
-  </si>
-  <si>
-    <t>Application closed.</t>
-  </si>
-  <si>
-    <t>Приложение закрыто.</t>
-  </si>
-  <si>
-    <t>SID_Versions_do_not_match</t>
-  </si>
-  <si>
-    <t>Client's version does not match server's one!</t>
-  </si>
-  <si>
-    <t>Версия клиента не совпадает с версией сервера</t>
-  </si>
-  <si>
-    <t>SID_Please_close_browser</t>
-  </si>
-  <si>
-    <t>Please close browser's tab and start Fibertest again.</t>
-  </si>
-  <si>
-    <t>Пожалуйста, закройте вкладку браузера и повторите подключение в новой вкладке.</t>
-  </si>
-  <si>
-    <t>{{0}} without name</t>
+    <t>SID_There_is_a_TCE_with_the_same_name</t>
+  </si>
+  <si>
+    <t>There is a TCE with the same name</t>
+  </si>
+  <si>
+    <t>Существует TCE с таким же названием</t>
+  </si>
+  <si>
+    <t>SID_There_is_a_TCE_with_the_same_IP_address</t>
+  </si>
+  <si>
+    <t>There is a TCE with the same IP address</t>
+  </si>
+  <si>
+    <t>Существует TCE с таким же IP адресом</t>
+  </si>
+  <si>
+    <t>SID_ThresholdsAttention</t>
+  </si>
+  <si>
+    <t>Attention! The specified thresholds must be greater than the maximum values ​​in the inclusions on the trace</t>
+  </si>
+  <si>
+    <t>Внимание! Заданные пороги должны быть больше максимальных значений в неоднородностях на трассе</t>
+  </si>
+  <si>
+    <t>SID_Current_operation</t>
+  </si>
+  <si>
+    <t>Current operation</t>
+  </si>
+  <si>
+    <t>Текущая операция</t>
+  </si>
+  <si>
+    <t>SID_Operations_result</t>
+  </si>
+  <si>
+    <t>Operations result</t>
+  </si>
+  <si>
+    <t>Результаты операций</t>
+  </si>
+  <si>
+    <t>SID_Unauthorized_RTU_access</t>
+  </si>
+  <si>
+    <t>Unauthorized RTU access</t>
+  </si>
+  <si>
+    <t>Неавторизованный доступ к RTU</t>
+  </si>
+  <si>
+    <t>SID_Unauthorized_access_to_RTU__0__</t>
+  </si>
+  <si>
+    <t>SID_Please_enter_Platform_serial_number</t>
+  </si>
+  <si>
+    <t>Please enter Platform serial number</t>
+  </si>
+  <si>
+    <t>Пожалуйста, введите Серийный номер платформы</t>
+  </si>
+  <si>
+    <t>SID_Continue</t>
+  </si>
+  <si>
+    <t>Continue</t>
+  </si>
+  <si>
+    <t>Продолжить</t>
+  </si>
+  <si>
+    <t>SID_Initialize_and_synch</t>
+  </si>
+  <si>
+    <t>Initialize RTU and Synchronize base refs</t>
+  </si>
+  <si>
+    <t>Инициализировать RTU и синхронизировать базовые</t>
+  </si>
+  <si>
+    <t>SID_Sending_base_refs_for_port__0_</t>
+  </si>
+  <si>
+    <t>SID_Iit_address</t>
+  </si>
+  <si>
+    <t>220099, the Republic of Belarus, Minsk, Kazintsa st., 11A, office 304a</t>
+  </si>
+  <si>
+    <t>220099, Республика Беларусь, г. Минск, ул. Казинца, д. 11а, офис 304а</t>
+  </si>
+  <si>
+    <t>SID_Iit_Phone</t>
+  </si>
+  <si>
+    <t>Phone:  +375 17 2359048</t>
+  </si>
+  <si>
+    <t>Телефон: +375 17 2359048</t>
+  </si>
+  <si>
+    <t>SID_All_rights_reserved</t>
+  </si>
+  <si>
+    <t>All rights reserved</t>
+  </si>
+  <si>
+    <t>Все права защищены</t>
+  </si>
+  <si>
+    <t>SID_Optical_km</t>
+  </si>
+  <si>
+    <t>Optical, km</t>
+  </si>
+  <si>
+    <t>Оптич, км</t>
+  </si>
+  <si>
+    <t>SID_Gps_km</t>
+  </si>
+  <si>
+    <t>GPS, km</t>
+  </si>
+  <si>
+    <t>GPS, км</t>
+  </si>
+  <si>
+    <t>SID_Cable_reserve_m</t>
+  </si>
+  <si>
+    <t>Cable reserve, m</t>
+  </si>
+  <si>
+    <t>Запас кабеля, м</t>
+  </si>
+  <si>
+    <t>SID_Gps_section_km</t>
+  </si>
+  <si>
+    <t>GPS section, km</t>
+  </si>
+  <si>
+    <t>Участок по GPS, км</t>
+  </si>
+  <si>
+    <t>SID_Optical_section_km</t>
+  </si>
+  <si>
+    <t>Optical section, km</t>
+  </si>
+  <si>
+    <t>Оптический участок, км</t>
+  </si>
+  <si>
+    <t>SID_Edit_node</t>
+  </si>
+  <si>
+    <t>Edit node</t>
+  </si>
+  <si>
+    <t>Редактировать узел</t>
+  </si>
+  <si>
+    <t>SID_Edit_fiber</t>
+  </si>
+  <si>
+    <t>Edit fiber</t>
+  </si>
+  <si>
+    <t>Редактировать участок</t>
   </si>
   <si>
     <t>{{0}} без имени</t>
@@ -9973,16 +9931,244 @@
     <t>RTU {{0}} занят.</t>
   </si>
   <si>
+    <t>Unauthorized access to RTU {{0}}.</t>
+  </si>
+  <si>
+    <t>Неавторизованный доступ к RTU {{0}}.</t>
+  </si>
+  <si>
+    <t>Sending base refs for port {{0}}</t>
+  </si>
+  <si>
+    <t>Пересылка базовых для порта {{0}}</t>
+  </si>
+  <si>
+    <t>en-US</t>
+  </si>
+  <si>
+    <t>ru-RU</t>
+  </si>
+  <si>
+    <t>SID_Items_per_page</t>
+  </si>
+  <si>
+    <t>Items per page</t>
+  </si>
+  <si>
+    <t>Строк на странице</t>
+  </si>
+  <si>
+    <t>SID_Next_page</t>
+  </si>
+  <si>
+    <t>Next page</t>
+  </si>
+  <si>
+    <t>Следующая страница</t>
+  </si>
+  <si>
+    <t>SID_Previous_page</t>
+  </si>
+  <si>
+    <t>Previous page</t>
+  </si>
+  <si>
+    <t>Предыдущая страница</t>
+  </si>
+  <si>
+    <t>SID_of</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> of </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> из </t>
+  </si>
+  <si>
+    <t>SID_Responsive</t>
+  </si>
+  <si>
+    <t>Responsive</t>
+  </si>
+  <si>
+    <t>Отзывчивый</t>
+  </si>
+  <si>
+    <t>SID_Rtu_Moni_Settings</t>
+  </si>
+  <si>
     <t xml:space="preserve">{{0}}: Monitoring Settings </t>
   </si>
   <si>
+    <t>{{0}}:  Настройки мониторинга</t>
+  </si>
+  <si>
+    <t>SID_measurement_frequency</t>
+  </si>
+  <si>
+    <t>measurement frequency</t>
+  </si>
+  <si>
+    <t>частота измерений</t>
+  </si>
+  <si>
+    <t>SID_saving_frequency</t>
+  </si>
+  <si>
+    <t>saving frequency</t>
+  </si>
+  <si>
+    <t>частота сохранения</t>
+  </si>
+  <si>
+    <t>SID_Cycle_full_time_sec</t>
+  </si>
+  <si>
     <t>Cycle full time {{0}} sec</t>
   </si>
   <si>
-    <t>{{0}}:  Настройки мониторинга</t>
-  </si>
-  <si>
     <t>Полное время цикла {{0}} сек</t>
+  </si>
+  <si>
+    <t>SID_Auto</t>
+  </si>
+  <si>
+    <t>Авто</t>
+  </si>
+  <si>
+    <t>SID_Landmark_count_does_not_match_graph</t>
+  </si>
+  <si>
+    <t>Landmark count on base ref does not match graph</t>
+  </si>
+  <si>
+    <t>Количество ориентиров на рефлектограмме не соответствует графу</t>
+  </si>
+  <si>
+    <t>Attach optical switch</t>
+  </si>
+  <si>
+    <t>Подключить оптический переключатель</t>
+  </si>
+  <si>
+    <t>SID_Optical_switch_s_IP_address</t>
+  </si>
+  <si>
+    <t>Optical switch's IP address</t>
+  </si>
+  <si>
+    <t>IP адрес оптического переключателя</t>
+  </si>
+  <si>
+    <t>SID_Web_Client_software_version</t>
+  </si>
+  <si>
+    <t>Web-Client software version</t>
+  </si>
+  <si>
+    <t>Версия ПК WebClient</t>
+  </si>
+  <si>
+    <t>SID_Web_Api_software_version</t>
+  </si>
+  <si>
+    <t>Web API software version</t>
+  </si>
+  <si>
+    <t>Верия ПК Web API</t>
+  </si>
+  <si>
+    <t>SID_Save_reflectogram</t>
+  </si>
+  <si>
+    <t>Save reflectogram</t>
+  </si>
+  <si>
+    <t>Сохранить рефлектограмму</t>
+  </si>
+  <si>
+    <t>SID_Save_ref_and_base</t>
+  </si>
+  <si>
+    <t>Save ref + base</t>
+  </si>
+  <si>
+    <t>Сохранить рефлектограмму + базовую</t>
+  </si>
+  <si>
+    <t>SID_Logout</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Выйти</t>
+  </si>
+  <si>
+    <t>SID_RTU_Tree</t>
+  </si>
+  <si>
+    <t>RTUs</t>
+  </si>
+  <si>
+    <t>Модули</t>
+  </si>
+  <si>
+    <t>SID_Reject</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>Отклонить</t>
+  </si>
+  <si>
+    <t>SID_Yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Да</t>
+  </si>
+  <si>
+    <t>SID_No</t>
+  </si>
+  <si>
+    <t>SID_Device</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Устройство</t>
+  </si>
+  <si>
+    <t>SID_Application_closed</t>
+  </si>
+  <si>
+    <t>Application closed.</t>
+  </si>
+  <si>
+    <t>Приложение закрыто.</t>
+  </si>
+  <si>
+    <t>SID_Versions_do_not_match</t>
+  </si>
+  <si>
+    <t>Client's version does not match server's one!</t>
+  </si>
+  <si>
+    <t>Версия клиента не совпадает с версией сервера</t>
+  </si>
+  <si>
+    <t>SID_Please_close_browser</t>
+  </si>
+  <si>
+    <t>Please close browser's tab and start Fibertest again.</t>
+  </si>
+  <si>
+    <t>Пожалуйста, закройте вкладку браузера и повторите подключение в новой вкладке.</t>
   </si>
 </sst>
 </file>
@@ -10042,7 +10228,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -10065,7 +10255,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{2724B5CE-EA8B-4F35-99AA-1909AD3275B3}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{EA2CA503-63F4-4FDA-864F-6D7DC7B1698C}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -10092,7 +10282,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{BE1CCAA9-EACA-482A-8BE0-0C2A4791B817}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{89DFD66E-20F5-4815-9697-4EC48308C5E6}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -10405,28 +10595,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1121"/>
+  <dimension ref="A1:C1142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1103" workbookViewId="0">
-      <selection activeCell="C1105" sqref="C1105"/>
+    <sheetView tabSelected="1" topLeftCell="A1111" workbookViewId="0">
+      <selection activeCell="D1121" sqref="D1121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.85546875" customWidth="1"/>
-    <col min="2" max="2" width="99.28515625" customWidth="1"/>
-    <col min="3" max="3" width="243.140625" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52" customWidth="1"/>
+    <col min="3" max="3" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2978</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2979</v>
+      <c r="B1" t="s">
+        <v>3303</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3304</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -10863,10 +11053,10 @@
         <v>118</v>
       </c>
       <c r="B41" t="s">
-        <v>3050</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>3051</v>
+        <v>3037</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -10896,10 +11086,10 @@
         <v>125</v>
       </c>
       <c r="B44" t="s">
-        <v>3052</v>
+        <v>3038</v>
       </c>
       <c r="C44" t="s">
-        <v>3052</v>
+        <v>3038</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -10907,10 +11097,10 @@
         <v>126</v>
       </c>
       <c r="B45" t="s">
-        <v>3053</v>
+        <v>3039</v>
       </c>
       <c r="C45" t="s">
-        <v>3054</v>
+        <v>3040</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -11149,10 +11339,10 @@
         <v>190</v>
       </c>
       <c r="B67" t="s">
-        <v>3055</v>
+        <v>3041</v>
       </c>
       <c r="C67" t="s">
-        <v>3055</v>
+        <v>3041</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -11754,10 +11944,10 @@
         <v>353</v>
       </c>
       <c r="B122" t="s">
-        <v>3056</v>
+        <v>3042</v>
       </c>
       <c r="C122" t="s">
-        <v>3057</v>
+        <v>3043</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -11765,10 +11955,10 @@
         <v>354</v>
       </c>
       <c r="B123" t="s">
-        <v>3058</v>
+        <v>3044</v>
       </c>
       <c r="C123" t="s">
-        <v>3059</v>
+        <v>3045</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -12139,10 +12329,10 @@
         <v>449</v>
       </c>
       <c r="B157" t="s">
-        <v>3060</v>
+        <v>3046</v>
       </c>
       <c r="C157" t="s">
-        <v>3060</v>
+        <v>3046</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -12381,10 +12571,10 @@
         <v>511</v>
       </c>
       <c r="B179" t="s">
-        <v>3061</v>
+        <v>3047</v>
       </c>
       <c r="C179" t="s">
-        <v>3062</v>
+        <v>3048</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -12821,10 +13011,10 @@
         <v>629</v>
       </c>
       <c r="B219" t="s">
-        <v>3063</v>
+        <v>3049</v>
       </c>
       <c r="C219" t="s">
-        <v>3064</v>
+        <v>3050</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
@@ -12865,10 +13055,10 @@
         <v>639</v>
       </c>
       <c r="B223" t="s">
-        <v>3065</v>
+        <v>3051</v>
       </c>
       <c r="C223" t="s">
-        <v>3066</v>
+        <v>3052</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -12876,10 +13066,10 @@
         <v>640</v>
       </c>
       <c r="B224" t="s">
-        <v>3067</v>
+        <v>3053</v>
       </c>
       <c r="C224" t="s">
-        <v>3068</v>
+        <v>3054</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -12920,10 +13110,10 @@
         <v>650</v>
       </c>
       <c r="B228" t="s">
-        <v>3069</v>
+        <v>3055</v>
       </c>
       <c r="C228" t="s">
-        <v>3070</v>
+        <v>3056</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -12931,10 +13121,10 @@
         <v>651</v>
       </c>
       <c r="B229" t="s">
-        <v>3071</v>
+        <v>3057</v>
       </c>
       <c r="C229" t="s">
-        <v>3072</v>
+        <v>3058</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -12964,10 +13154,10 @@
         <v>657</v>
       </c>
       <c r="B232" t="s">
-        <v>3073</v>
+        <v>3059</v>
       </c>
       <c r="C232" t="s">
-        <v>3073</v>
+        <v>3059</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -13008,10 +13198,10 @@
         <v>664</v>
       </c>
       <c r="B236" t="s">
-        <v>3074</v>
+        <v>3060</v>
       </c>
       <c r="C236" t="s">
-        <v>3074</v>
+        <v>3060</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -13019,10 +13209,10 @@
         <v>665</v>
       </c>
       <c r="B237" t="s">
-        <v>3075</v>
+        <v>3061</v>
       </c>
       <c r="C237" t="s">
-        <v>3075</v>
+        <v>3061</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -13030,10 +13220,10 @@
         <v>666</v>
       </c>
       <c r="B238" t="s">
-        <v>3076</v>
+        <v>3062</v>
       </c>
       <c r="C238" t="s">
-        <v>3076</v>
+        <v>3062</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -13074,10 +13264,10 @@
         <v>674</v>
       </c>
       <c r="B242" t="s">
-        <v>3077</v>
+        <v>3063</v>
       </c>
       <c r="C242" t="s">
-        <v>3077</v>
+        <v>3063</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
@@ -13283,10 +13473,10 @@
         <v>729</v>
       </c>
       <c r="B261" t="s">
-        <v>3078</v>
+        <v>3064</v>
       </c>
       <c r="C261" t="s">
-        <v>3079</v>
+        <v>3065</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -13294,10 +13484,10 @@
         <v>730</v>
       </c>
       <c r="B262" t="s">
-        <v>3080</v>
+        <v>3066</v>
       </c>
       <c r="C262" t="s">
-        <v>3081</v>
+        <v>3067</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -13305,10 +13495,10 @@
         <v>731</v>
       </c>
       <c r="B263" t="s">
-        <v>3082</v>
+        <v>3068</v>
       </c>
       <c r="C263" t="s">
-        <v>3083</v>
+        <v>3069</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -13316,10 +13506,10 @@
         <v>732</v>
       </c>
       <c r="B264" t="s">
-        <v>3084</v>
+        <v>3070</v>
       </c>
       <c r="C264" t="s">
-        <v>3085</v>
+        <v>3071</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -13404,10 +13594,10 @@
         <v>754</v>
       </c>
       <c r="B272" t="s">
-        <v>3086</v>
+        <v>3072</v>
       </c>
       <c r="C272" t="s">
-        <v>3087</v>
+        <v>3073</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -13415,10 +13605,10 @@
         <v>755</v>
       </c>
       <c r="B273" t="s">
-        <v>3088</v>
+        <v>3074</v>
       </c>
       <c r="C273" t="s">
-        <v>3089</v>
+        <v>3075</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -13426,10 +13616,10 @@
         <v>756</v>
       </c>
       <c r="B274" t="s">
-        <v>3090</v>
+        <v>3076</v>
       </c>
       <c r="C274" t="s">
-        <v>3091</v>
+        <v>3077</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -13723,10 +13913,10 @@
         <v>835</v>
       </c>
       <c r="B301" t="s">
-        <v>3092</v>
+        <v>3078</v>
       </c>
       <c r="C301" t="s">
-        <v>3093</v>
+        <v>3079</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
@@ -13734,10 +13924,10 @@
         <v>836</v>
       </c>
       <c r="B302" t="s">
-        <v>3094</v>
+        <v>3080</v>
       </c>
       <c r="C302" t="s">
-        <v>3095</v>
+        <v>3081</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
@@ -13822,10 +14012,10 @@
         <v>858</v>
       </c>
       <c r="B310" t="s">
-        <v>3096</v>
+        <v>3082</v>
       </c>
       <c r="C310" t="s">
-        <v>3097</v>
+        <v>3083</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -13833,10 +14023,10 @@
         <v>859</v>
       </c>
       <c r="B311" t="s">
-        <v>3098</v>
+        <v>3084</v>
       </c>
       <c r="C311" t="s">
-        <v>3099</v>
+        <v>3085</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -13844,10 +14034,10 @@
         <v>860</v>
       </c>
       <c r="B312" t="s">
-        <v>3100</v>
+        <v>3086</v>
       </c>
       <c r="C312" t="s">
-        <v>3101</v>
+        <v>3087</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -13855,10 +14045,10 @@
         <v>861</v>
       </c>
       <c r="B313" t="s">
-        <v>3102</v>
+        <v>3088</v>
       </c>
       <c r="C313" t="s">
-        <v>3103</v>
+        <v>3089</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -13976,10 +14166,10 @@
         <v>892</v>
       </c>
       <c r="B324" t="s">
-        <v>3104</v>
+        <v>3090</v>
       </c>
       <c r="C324" t="s">
-        <v>3105</v>
+        <v>3091</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -14020,10 +14210,10 @@
         <v>902</v>
       </c>
       <c r="B328" t="s">
-        <v>3106</v>
+        <v>3092</v>
       </c>
       <c r="C328" t="s">
-        <v>3107</v>
+        <v>3093</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
@@ -14042,10 +14232,10 @@
         <v>906</v>
       </c>
       <c r="B330" t="s">
-        <v>3108</v>
+        <v>3094</v>
       </c>
       <c r="C330" t="s">
-        <v>3109</v>
+        <v>3095</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
@@ -14570,10 +14760,10 @@
         <v>1048</v>
       </c>
       <c r="B378" t="s">
-        <v>3110</v>
+        <v>3096</v>
       </c>
       <c r="C378" t="s">
-        <v>3111</v>
+        <v>3097</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
@@ -14933,10 +15123,10 @@
         <v>1144</v>
       </c>
       <c r="B411" t="s">
-        <v>3112</v>
+        <v>3098</v>
       </c>
       <c r="C411" t="s">
-        <v>3113</v>
+        <v>3099</v>
       </c>
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.25">
@@ -14944,10 +15134,10 @@
         <v>1145</v>
       </c>
       <c r="B412" t="s">
-        <v>3114</v>
+        <v>3100</v>
       </c>
       <c r="C412" t="s">
-        <v>3115</v>
+        <v>3101</v>
       </c>
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
@@ -14955,10 +15145,10 @@
         <v>1146</v>
       </c>
       <c r="B413" t="s">
-        <v>3116</v>
+        <v>3102</v>
       </c>
       <c r="C413" t="s">
-        <v>3117</v>
+        <v>3103</v>
       </c>
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.25">
@@ -14977,10 +15167,10 @@
         <v>1150</v>
       </c>
       <c r="B415" t="s">
-        <v>3118</v>
+        <v>3104</v>
       </c>
       <c r="C415" t="s">
-        <v>3119</v>
+        <v>3105</v>
       </c>
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
@@ -15010,10 +15200,10 @@
         <v>1157</v>
       </c>
       <c r="B418" t="s">
-        <v>3120</v>
+        <v>3106</v>
       </c>
       <c r="C418" t="s">
-        <v>3121</v>
+        <v>3107</v>
       </c>
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
@@ -15120,10 +15310,10 @@
         <v>1185</v>
       </c>
       <c r="B428" t="s">
-        <v>3122</v>
+        <v>3108</v>
       </c>
       <c r="C428" t="s">
-        <v>3123</v>
+        <v>3109</v>
       </c>
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
@@ -15131,10 +15321,10 @@
         <v>1186</v>
       </c>
       <c r="B429" t="s">
-        <v>3124</v>
+        <v>3110</v>
       </c>
       <c r="C429" t="s">
-        <v>3125</v>
+        <v>3111</v>
       </c>
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
@@ -15153,10 +15343,10 @@
         <v>1190</v>
       </c>
       <c r="B431" t="s">
-        <v>3126</v>
+        <v>3112</v>
       </c>
       <c r="C431" t="s">
-        <v>3127</v>
+        <v>3113</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
@@ -15164,10 +15354,10 @@
         <v>1191</v>
       </c>
       <c r="B432" t="s">
-        <v>3128</v>
+        <v>3114</v>
       </c>
       <c r="C432" t="s">
-        <v>3129</v>
+        <v>3115</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
@@ -15285,10 +15475,10 @@
         <v>1222</v>
       </c>
       <c r="B443" t="s">
-        <v>3130</v>
+        <v>3116</v>
       </c>
       <c r="C443" t="s">
-        <v>3131</v>
+        <v>3117</v>
       </c>
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.25">
@@ -15296,10 +15486,10 @@
         <v>1223</v>
       </c>
       <c r="B444" t="s">
-        <v>3132</v>
+        <v>3118</v>
       </c>
       <c r="C444" t="s">
-        <v>3133</v>
+        <v>3119</v>
       </c>
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.25">
@@ -15318,10 +15508,10 @@
         <v>1227</v>
       </c>
       <c r="B446" t="s">
-        <v>3134</v>
+        <v>3120</v>
       </c>
       <c r="C446" t="s">
-        <v>3135</v>
+        <v>3121</v>
       </c>
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.25">
@@ -15329,10 +15519,10 @@
         <v>1228</v>
       </c>
       <c r="B447" t="s">
-        <v>3136</v>
+        <v>3122</v>
       </c>
       <c r="C447" t="s">
-        <v>3137</v>
+        <v>3123</v>
       </c>
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
@@ -15439,10 +15629,10 @@
         <v>1256</v>
       </c>
       <c r="B457" t="s">
-        <v>3138</v>
+        <v>3124</v>
       </c>
       <c r="C457" t="s">
-        <v>3139</v>
+        <v>3125</v>
       </c>
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.25">
@@ -15450,10 +15640,10 @@
         <v>1257</v>
       </c>
       <c r="B458" t="s">
-        <v>3140</v>
+        <v>3126</v>
       </c>
       <c r="C458" t="s">
-        <v>3141</v>
+        <v>3127</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.25">
@@ -15582,10 +15772,10 @@
         <v>1291</v>
       </c>
       <c r="B470" t="s">
-        <v>3142</v>
+        <v>3128</v>
       </c>
       <c r="C470" t="s">
-        <v>3143</v>
+        <v>3129</v>
       </c>
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.25">
@@ -15912,10 +16102,10 @@
         <v>1378</v>
       </c>
       <c r="B500" t="s">
-        <v>3144</v>
+        <v>3130</v>
       </c>
       <c r="C500" t="s">
-        <v>3145</v>
+        <v>3131</v>
       </c>
     </row>
     <row r="501" spans="1:3" x14ac:dyDescent="0.25">
@@ -15923,10 +16113,10 @@
         <v>1379</v>
       </c>
       <c r="B501" t="s">
-        <v>3146</v>
+        <v>3132</v>
       </c>
       <c r="C501" t="s">
-        <v>3147</v>
+        <v>3133</v>
       </c>
     </row>
     <row r="502" spans="1:3" x14ac:dyDescent="0.25">
@@ -16000,10 +16190,10 @@
         <v>1398</v>
       </c>
       <c r="B508" t="s">
-        <v>3148</v>
+        <v>3134</v>
       </c>
       <c r="C508" t="s">
-        <v>3149</v>
+        <v>3135</v>
       </c>
     </row>
     <row r="509" spans="1:3" x14ac:dyDescent="0.25">
@@ -16374,10 +16564,10 @@
         <v>1496</v>
       </c>
       <c r="B542" t="s">
-        <v>3150</v>
+        <v>3136</v>
       </c>
       <c r="C542" t="s">
-        <v>3151</v>
+        <v>3137</v>
       </c>
     </row>
     <row r="543" spans="1:3" x14ac:dyDescent="0.25">
@@ -16418,10 +16608,10 @@
         <v>1506</v>
       </c>
       <c r="B546" t="s">
-        <v>3152</v>
+        <v>3138</v>
       </c>
       <c r="C546" t="s">
-        <v>3153</v>
+        <v>3139</v>
       </c>
     </row>
     <row r="547" spans="1:3" x14ac:dyDescent="0.25">
@@ -16803,10 +16993,10 @@
         <v>1609</v>
       </c>
       <c r="B581" t="s">
-        <v>3154</v>
+        <v>3140</v>
       </c>
       <c r="C581" t="s">
-        <v>3155</v>
+        <v>3141</v>
       </c>
     </row>
     <row r="582" spans="1:3" x14ac:dyDescent="0.25">
@@ -16891,10 +17081,10 @@
         <v>1631</v>
       </c>
       <c r="B589" t="s">
-        <v>3156</v>
+        <v>3142</v>
       </c>
       <c r="C589" t="s">
-        <v>3157</v>
+        <v>3143</v>
       </c>
     </row>
     <row r="590" spans="1:3" x14ac:dyDescent="0.25">
@@ -16913,10 +17103,10 @@
         <v>1635</v>
       </c>
       <c r="B591" t="s">
-        <v>3158</v>
+        <v>3144</v>
       </c>
       <c r="C591" t="s">
-        <v>3159</v>
+        <v>3145</v>
       </c>
     </row>
     <row r="592" spans="1:3" x14ac:dyDescent="0.25">
@@ -16968,10 +17158,10 @@
         <v>1648</v>
       </c>
       <c r="B596" t="s">
-        <v>3160</v>
+        <v>3146</v>
       </c>
       <c r="C596" t="s">
-        <v>3161</v>
+        <v>3147</v>
       </c>
     </row>
     <row r="597" spans="1:3" x14ac:dyDescent="0.25">
@@ -16979,10 +17169,10 @@
         <v>1649</v>
       </c>
       <c r="B597" t="s">
-        <v>3162</v>
+        <v>3148</v>
       </c>
       <c r="C597" t="s">
-        <v>3163</v>
+        <v>3149</v>
       </c>
     </row>
     <row r="598" spans="1:3" x14ac:dyDescent="0.25">
@@ -17001,10 +17191,10 @@
         <v>1653</v>
       </c>
       <c r="B599" t="s">
-        <v>3164</v>
+        <v>3150</v>
       </c>
       <c r="C599" t="s">
-        <v>3165</v>
+        <v>3151</v>
       </c>
     </row>
     <row r="600" spans="1:3" x14ac:dyDescent="0.25">
@@ -17012,10 +17202,10 @@
         <v>1654</v>
       </c>
       <c r="B600" t="s">
-        <v>3166</v>
+        <v>3152</v>
       </c>
       <c r="C600" t="s">
-        <v>3167</v>
+        <v>3153</v>
       </c>
     </row>
     <row r="601" spans="1:3" x14ac:dyDescent="0.25">
@@ -17023,10 +17213,10 @@
         <v>1655</v>
       </c>
       <c r="B601" t="s">
-        <v>3168</v>
+        <v>3154</v>
       </c>
       <c r="C601" t="s">
-        <v>3169</v>
+        <v>3155</v>
       </c>
     </row>
     <row r="602" spans="1:3" x14ac:dyDescent="0.25">
@@ -17034,10 +17224,10 @@
         <v>1656</v>
       </c>
       <c r="B602" t="s">
-        <v>3170</v>
+        <v>3156</v>
       </c>
       <c r="C602" t="s">
-        <v>3171</v>
+        <v>3157</v>
       </c>
     </row>
     <row r="603" spans="1:3" x14ac:dyDescent="0.25">
@@ -17100,10 +17290,10 @@
         <v>1672</v>
       </c>
       <c r="B608" t="s">
-        <v>3172</v>
+        <v>3158</v>
       </c>
       <c r="C608" t="s">
-        <v>3173</v>
+        <v>3159</v>
       </c>
     </row>
     <row r="609" spans="1:3" x14ac:dyDescent="0.25">
@@ -17122,10 +17312,10 @@
         <v>1676</v>
       </c>
       <c r="B610" t="s">
-        <v>3174</v>
+        <v>3160</v>
       </c>
       <c r="C610" t="s">
-        <v>3175</v>
+        <v>3161</v>
       </c>
     </row>
     <row r="611" spans="1:3" x14ac:dyDescent="0.25">
@@ -17166,10 +17356,10 @@
         <v>1686</v>
       </c>
       <c r="B614" t="s">
-        <v>3176</v>
+        <v>3162</v>
       </c>
       <c r="C614" t="s">
-        <v>3177</v>
+        <v>3163</v>
       </c>
     </row>
     <row r="615" spans="1:3" x14ac:dyDescent="0.25">
@@ -17188,10 +17378,10 @@
         <v>1690</v>
       </c>
       <c r="B616" t="s">
-        <v>3178</v>
+        <v>3164</v>
       </c>
       <c r="C616" t="s">
-        <v>3179</v>
+        <v>3165</v>
       </c>
     </row>
     <row r="617" spans="1:3" x14ac:dyDescent="0.25">
@@ -17199,10 +17389,10 @@
         <v>1691</v>
       </c>
       <c r="B617" t="s">
-        <v>3180</v>
+        <v>3166</v>
       </c>
       <c r="C617" t="s">
-        <v>3181</v>
+        <v>3167</v>
       </c>
     </row>
     <row r="618" spans="1:3" x14ac:dyDescent="0.25">
@@ -17221,10 +17411,10 @@
         <v>1695</v>
       </c>
       <c r="B619" t="s">
-        <v>3182</v>
+        <v>3168</v>
       </c>
       <c r="C619" t="s">
-        <v>3183</v>
+        <v>3169</v>
       </c>
     </row>
     <row r="620" spans="1:3" x14ac:dyDescent="0.25">
@@ -17232,10 +17422,10 @@
         <v>1696</v>
       </c>
       <c r="B620" t="s">
-        <v>3184</v>
+        <v>3170</v>
       </c>
       <c r="C620" t="s">
-        <v>3185</v>
+        <v>3171</v>
       </c>
     </row>
     <row r="621" spans="1:3" x14ac:dyDescent="0.25">
@@ -17342,10 +17532,10 @@
         <v>1723</v>
       </c>
       <c r="B630" t="s">
-        <v>3186</v>
+        <v>3172</v>
       </c>
       <c r="C630" t="s">
-        <v>3187</v>
+        <v>3173</v>
       </c>
     </row>
     <row r="631" spans="1:3" x14ac:dyDescent="0.25">
@@ -17353,10 +17543,10 @@
         <v>1724</v>
       </c>
       <c r="B631" t="s">
-        <v>3188</v>
+        <v>3174</v>
       </c>
       <c r="C631" t="s">
-        <v>3189</v>
+        <v>3175</v>
       </c>
     </row>
     <row r="632" spans="1:3" x14ac:dyDescent="0.25">
@@ -17375,10 +17565,10 @@
         <v>1728</v>
       </c>
       <c r="B633" t="s">
-        <v>3190</v>
+        <v>3176</v>
       </c>
       <c r="C633" t="s">
-        <v>3191</v>
+        <v>3177</v>
       </c>
     </row>
     <row r="634" spans="1:3" x14ac:dyDescent="0.25">
@@ -17386,10 +17576,10 @@
         <v>1729</v>
       </c>
       <c r="B634" t="s">
-        <v>3192</v>
+        <v>3178</v>
       </c>
       <c r="C634" t="s">
-        <v>3193</v>
+        <v>3179</v>
       </c>
     </row>
     <row r="635" spans="1:3" x14ac:dyDescent="0.25">
@@ -17397,10 +17587,10 @@
         <v>1730</v>
       </c>
       <c r="B635" t="s">
-        <v>3194</v>
+        <v>3180</v>
       </c>
       <c r="C635" t="s">
-        <v>3195</v>
+        <v>3181</v>
       </c>
     </row>
     <row r="636" spans="1:3" x14ac:dyDescent="0.25">
@@ -17408,10 +17598,10 @@
         <v>1731</v>
       </c>
       <c r="B636" t="s">
-        <v>3196</v>
+        <v>3182</v>
       </c>
       <c r="C636" t="s">
-        <v>3197</v>
+        <v>3183</v>
       </c>
     </row>
     <row r="637" spans="1:3" x14ac:dyDescent="0.25">
@@ -17419,10 +17609,10 @@
         <v>1732</v>
       </c>
       <c r="B637" t="s">
-        <v>3198</v>
+        <v>3184</v>
       </c>
       <c r="C637" t="s">
-        <v>3199</v>
+        <v>3185</v>
       </c>
     </row>
     <row r="638" spans="1:3" x14ac:dyDescent="0.25">
@@ -17430,10 +17620,10 @@
         <v>1733</v>
       </c>
       <c r="B638" t="s">
-        <v>3200</v>
+        <v>3186</v>
       </c>
       <c r="C638" t="s">
-        <v>3201</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="639" spans="1:3" x14ac:dyDescent="0.25">
@@ -17441,10 +17631,10 @@
         <v>1734</v>
       </c>
       <c r="B639" t="s">
-        <v>3202</v>
+        <v>3188</v>
       </c>
       <c r="C639" t="s">
-        <v>3203</v>
+        <v>3189</v>
       </c>
     </row>
     <row r="640" spans="1:3" x14ac:dyDescent="0.25">
@@ -17452,10 +17642,10 @@
         <v>1735</v>
       </c>
       <c r="B640" t="s">
-        <v>3204</v>
+        <v>3190</v>
       </c>
       <c r="C640" t="s">
-        <v>3205</v>
+        <v>3191</v>
       </c>
     </row>
     <row r="641" spans="1:3" x14ac:dyDescent="0.25">
@@ -17463,10 +17653,10 @@
         <v>1736</v>
       </c>
       <c r="B641" t="s">
-        <v>3206</v>
+        <v>3192</v>
       </c>
       <c r="C641" t="s">
-        <v>3207</v>
+        <v>3193</v>
       </c>
     </row>
     <row r="642" spans="1:3" x14ac:dyDescent="0.25">
@@ -17815,10 +18005,10 @@
         <v>1830</v>
       </c>
       <c r="B673" t="s">
-        <v>3208</v>
+        <v>3194</v>
       </c>
       <c r="C673" t="s">
-        <v>3209</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="674" spans="1:3" x14ac:dyDescent="0.25">
@@ -17848,10 +18038,10 @@
         <v>1837</v>
       </c>
       <c r="B676" t="s">
-        <v>3210</v>
+        <v>3196</v>
       </c>
       <c r="C676" t="s">
-        <v>3211</v>
+        <v>3197</v>
       </c>
     </row>
     <row r="677" spans="1:3" x14ac:dyDescent="0.25">
@@ -17859,10 +18049,10 @@
         <v>1838</v>
       </c>
       <c r="B677" t="s">
-        <v>3212</v>
+        <v>3198</v>
       </c>
       <c r="C677" t="s">
-        <v>3213</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="678" spans="1:3" x14ac:dyDescent="0.25">
@@ -17870,10 +18060,10 @@
         <v>1839</v>
       </c>
       <c r="B678" t="s">
-        <v>3214</v>
+        <v>3200</v>
       </c>
       <c r="C678" t="s">
-        <v>3215</v>
+        <v>3201</v>
       </c>
     </row>
     <row r="679" spans="1:3" x14ac:dyDescent="0.25">
@@ -17881,10 +18071,10 @@
         <v>1840</v>
       </c>
       <c r="B679" t="s">
-        <v>3216</v>
+        <v>3202</v>
       </c>
       <c r="C679" t="s">
-        <v>3217</v>
+        <v>3203</v>
       </c>
     </row>
     <row r="680" spans="1:3" x14ac:dyDescent="0.25">
@@ -17892,10 +18082,10 @@
         <v>1841</v>
       </c>
       <c r="B680" t="s">
-        <v>3218</v>
+        <v>3204</v>
       </c>
       <c r="C680" t="s">
-        <v>3219</v>
+        <v>3205</v>
       </c>
     </row>
     <row r="681" spans="1:3" x14ac:dyDescent="0.25">
@@ -17903,10 +18093,10 @@
         <v>1842</v>
       </c>
       <c r="B681" t="s">
-        <v>3220</v>
+        <v>3206</v>
       </c>
       <c r="C681" t="s">
-        <v>3221</v>
+        <v>3207</v>
       </c>
     </row>
     <row r="682" spans="1:3" x14ac:dyDescent="0.25">
@@ -18376,10 +18566,10 @@
         <v>1968</v>
       </c>
       <c r="B724" t="s">
-        <v>3222</v>
+        <v>3208</v>
       </c>
       <c r="C724" t="s">
-        <v>3223</v>
+        <v>3209</v>
       </c>
     </row>
     <row r="725" spans="1:3" x14ac:dyDescent="0.25">
@@ -18486,10 +18676,10 @@
         <v>1995</v>
       </c>
       <c r="B734" t="s">
-        <v>3224</v>
+        <v>3210</v>
       </c>
       <c r="C734" t="s">
-        <v>3225</v>
+        <v>3211</v>
       </c>
     </row>
     <row r="735" spans="1:3" x14ac:dyDescent="0.25">
@@ -18497,10 +18687,10 @@
         <v>1996</v>
       </c>
       <c r="B735" t="s">
-        <v>3226</v>
+        <v>3212</v>
       </c>
       <c r="C735" t="s">
-        <v>3227</v>
+        <v>3213</v>
       </c>
     </row>
     <row r="736" spans="1:3" x14ac:dyDescent="0.25">
@@ -18508,10 +18698,10 @@
         <v>1997</v>
       </c>
       <c r="B736" t="s">
-        <v>3228</v>
+        <v>3214</v>
       </c>
       <c r="C736" t="s">
-        <v>3229</v>
+        <v>3215</v>
       </c>
     </row>
     <row r="737" spans="1:3" x14ac:dyDescent="0.25">
@@ -18519,10 +18709,10 @@
         <v>1998</v>
       </c>
       <c r="B737" t="s">
-        <v>3230</v>
+        <v>3216</v>
       </c>
       <c r="C737" t="s">
-        <v>3231</v>
+        <v>3217</v>
       </c>
     </row>
     <row r="738" spans="1:3" x14ac:dyDescent="0.25">
@@ -18915,10 +19105,10 @@
         <v>2102</v>
       </c>
       <c r="B773" t="s">
-        <v>3232</v>
+        <v>3218</v>
       </c>
       <c r="C773" t="s">
-        <v>3233</v>
+        <v>3219</v>
       </c>
     </row>
     <row r="774" spans="1:3" x14ac:dyDescent="0.25">
@@ -18926,10 +19116,10 @@
         <v>2103</v>
       </c>
       <c r="B774" t="s">
-        <v>3234</v>
+        <v>3220</v>
       </c>
       <c r="C774" t="s">
-        <v>3235</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="775" spans="1:3" x14ac:dyDescent="0.25">
@@ -18937,10 +19127,10 @@
         <v>2104</v>
       </c>
       <c r="B775" t="s">
-        <v>3236</v>
+        <v>3222</v>
       </c>
       <c r="C775" t="s">
-        <v>3237</v>
+        <v>3223</v>
       </c>
     </row>
     <row r="776" spans="1:3" x14ac:dyDescent="0.25">
@@ -18948,10 +19138,10 @@
         <v>2105</v>
       </c>
       <c r="B776" t="s">
-        <v>3238</v>
+        <v>3224</v>
       </c>
       <c r="C776" t="s">
-        <v>3239</v>
+        <v>3225</v>
       </c>
     </row>
     <row r="777" spans="1:3" x14ac:dyDescent="0.25">
@@ -18959,10 +19149,10 @@
         <v>2106</v>
       </c>
       <c r="B777" t="s">
-        <v>3240</v>
+        <v>3226</v>
       </c>
       <c r="C777" t="s">
-        <v>3241</v>
+        <v>3227</v>
       </c>
     </row>
     <row r="778" spans="1:3" x14ac:dyDescent="0.25">
@@ -18992,10 +19182,10 @@
         <v>2113</v>
       </c>
       <c r="B780" t="s">
-        <v>3242</v>
+        <v>3228</v>
       </c>
       <c r="C780" t="s">
-        <v>3243</v>
+        <v>3229</v>
       </c>
     </row>
     <row r="781" spans="1:3" x14ac:dyDescent="0.25">
@@ -19003,10 +19193,10 @@
         <v>2114</v>
       </c>
       <c r="B781" t="s">
-        <v>3244</v>
+        <v>3230</v>
       </c>
       <c r="C781" t="s">
-        <v>3245</v>
+        <v>3231</v>
       </c>
     </row>
     <row r="782" spans="1:3" x14ac:dyDescent="0.25">
@@ -19135,10 +19325,10 @@
         <v>2148</v>
       </c>
       <c r="B793" t="s">
-        <v>3246</v>
+        <v>3232</v>
       </c>
       <c r="C793" t="s">
-        <v>3247</v>
+        <v>3233</v>
       </c>
     </row>
     <row r="794" spans="1:3" x14ac:dyDescent="0.25">
@@ -19157,10 +19347,10 @@
         <v>2152</v>
       </c>
       <c r="B795" t="s">
-        <v>3248</v>
+        <v>3234</v>
       </c>
       <c r="C795" t="s">
-        <v>3249</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="796" spans="1:3" x14ac:dyDescent="0.25">
@@ -19212,10 +19402,10 @@
         <v>2165</v>
       </c>
       <c r="B800" t="s">
-        <v>3250</v>
+        <v>3236</v>
       </c>
       <c r="C800" t="s">
-        <v>3250</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="801" spans="1:3" x14ac:dyDescent="0.25">
@@ -19223,10 +19413,10 @@
         <v>2166</v>
       </c>
       <c r="B801" t="s">
-        <v>3251</v>
+        <v>3237</v>
       </c>
       <c r="C801" t="s">
-        <v>3252</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="802" spans="1:3" x14ac:dyDescent="0.25">
@@ -19245,10 +19435,10 @@
         <v>2169</v>
       </c>
       <c r="B803" t="s">
-        <v>3253</v>
+        <v>3239</v>
       </c>
       <c r="C803" t="s">
-        <v>3254</v>
+        <v>3240</v>
       </c>
     </row>
     <row r="804" spans="1:3" x14ac:dyDescent="0.25">
@@ -19564,10 +19754,10 @@
         <v>2253</v>
       </c>
       <c r="B832" t="s">
-        <v>3255</v>
+        <v>3241</v>
       </c>
       <c r="C832" t="s">
-        <v>3256</v>
+        <v>3242</v>
       </c>
     </row>
     <row r="833" spans="1:3" x14ac:dyDescent="0.25">
@@ -19597,10 +19787,10 @@
         <v>2260</v>
       </c>
       <c r="B835" t="s">
-        <v>3257</v>
+        <v>3243</v>
       </c>
       <c r="C835" t="s">
-        <v>3258</v>
+        <v>3244</v>
       </c>
     </row>
     <row r="836" spans="1:3" x14ac:dyDescent="0.25">
@@ -19608,10 +19798,10 @@
         <v>2261</v>
       </c>
       <c r="B836" t="s">
-        <v>3259</v>
+        <v>3245</v>
       </c>
       <c r="C836" t="s">
-        <v>3260</v>
+        <v>3246</v>
       </c>
     </row>
     <row r="837" spans="1:3" x14ac:dyDescent="0.25">
@@ -19619,10 +19809,10 @@
         <v>2262</v>
       </c>
       <c r="B837" t="s">
-        <v>3261</v>
+        <v>3247</v>
       </c>
       <c r="C837" t="s">
-        <v>3262</v>
+        <v>3248</v>
       </c>
     </row>
     <row r="838" spans="1:3" x14ac:dyDescent="0.25">
@@ -19652,10 +19842,10 @@
         <v>2269</v>
       </c>
       <c r="B840" t="s">
-        <v>3263</v>
+        <v>3249</v>
       </c>
       <c r="C840" t="s">
-        <v>3264</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="841" spans="1:3" x14ac:dyDescent="0.25">
@@ -19839,10 +20029,10 @@
         <v>2318</v>
       </c>
       <c r="B857" t="s">
-        <v>3265</v>
+        <v>3251</v>
       </c>
       <c r="C857" t="s">
-        <v>3266</v>
+        <v>3252</v>
       </c>
     </row>
     <row r="858" spans="1:3" x14ac:dyDescent="0.25">
@@ -19872,10 +20062,10 @@
         <v>2325</v>
       </c>
       <c r="B860" t="s">
-        <v>3267</v>
+        <v>3253</v>
       </c>
       <c r="C860" t="s">
-        <v>3268</v>
+        <v>3254</v>
       </c>
     </row>
     <row r="861" spans="1:3" x14ac:dyDescent="0.25">
@@ -19883,10 +20073,10 @@
         <v>2326</v>
       </c>
       <c r="B861" t="s">
-        <v>3269</v>
+        <v>3255</v>
       </c>
       <c r="C861" t="s">
-        <v>3270</v>
+        <v>3256</v>
       </c>
     </row>
     <row r="862" spans="1:3" x14ac:dyDescent="0.25">
@@ -19894,10 +20084,10 @@
         <v>2327</v>
       </c>
       <c r="B862" t="s">
-        <v>3271</v>
+        <v>3257</v>
       </c>
       <c r="C862" t="s">
-        <v>3272</v>
+        <v>3258</v>
       </c>
     </row>
     <row r="863" spans="1:3" x14ac:dyDescent="0.25">
@@ -19905,10 +20095,10 @@
         <v>2328</v>
       </c>
       <c r="B863" t="s">
-        <v>3273</v>
+        <v>3259</v>
       </c>
       <c r="C863" t="s">
-        <v>3274</v>
+        <v>3260</v>
       </c>
     </row>
     <row r="864" spans="1:3" x14ac:dyDescent="0.25">
@@ -19916,10 +20106,10 @@
         <v>2329</v>
       </c>
       <c r="B864" t="s">
-        <v>3275</v>
+        <v>3261</v>
       </c>
       <c r="C864" t="s">
-        <v>3276</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="865" spans="1:3" x14ac:dyDescent="0.25">
@@ -20103,10 +20293,10 @@
         <v>2378</v>
       </c>
       <c r="B881" t="s">
-        <v>3277</v>
+        <v>3263</v>
       </c>
       <c r="C881" t="s">
-        <v>3278</v>
+        <v>3264</v>
       </c>
     </row>
     <row r="882" spans="1:3" x14ac:dyDescent="0.25">
@@ -20147,10 +20337,10 @@
         <v>2388</v>
       </c>
       <c r="B885" t="s">
-        <v>3279</v>
+        <v>3265</v>
       </c>
       <c r="C885" t="s">
-        <v>3280</v>
+        <v>3266</v>
       </c>
     </row>
     <row r="886" spans="1:3" x14ac:dyDescent="0.25">
@@ -20180,10 +20370,10 @@
         <v>2395</v>
       </c>
       <c r="B888" t="s">
-        <v>3281</v>
+        <v>3267</v>
       </c>
       <c r="C888" t="s">
-        <v>3282</v>
+        <v>3268</v>
       </c>
     </row>
     <row r="889" spans="1:3" x14ac:dyDescent="0.25">
@@ -20230,15 +20420,15 @@
         <v>2407</v>
       </c>
     </row>
-    <row r="893" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
         <v>2408</v>
       </c>
       <c r="B893" s="1" t="s">
-        <v>3283</v>
+        <v>3269</v>
       </c>
       <c r="C893" s="1" t="s">
-        <v>3284</v>
+        <v>3270</v>
       </c>
     </row>
     <row r="894" spans="1:3" x14ac:dyDescent="0.25">
@@ -20554,10 +20744,10 @@
         <v>2493</v>
       </c>
       <c r="B922" t="s">
-        <v>3285</v>
+        <v>3271</v>
       </c>
       <c r="C922" t="s">
-        <v>3286</v>
+        <v>3272</v>
       </c>
     </row>
     <row r="923" spans="1:3" x14ac:dyDescent="0.25">
@@ -20851,10 +21041,10 @@
         <v>2571</v>
       </c>
       <c r="B949" t="s">
-        <v>3287</v>
+        <v>3273</v>
       </c>
       <c r="C949" t="s">
-        <v>3288</v>
+        <v>3274</v>
       </c>
     </row>
     <row r="950" spans="1:3" x14ac:dyDescent="0.25">
@@ -20939,10 +21129,10 @@
         <v>2593</v>
       </c>
       <c r="B957" t="s">
-        <v>3289</v>
+        <v>3275</v>
       </c>
       <c r="C957" t="s">
-        <v>3290</v>
+        <v>3276</v>
       </c>
     </row>
     <row r="958" spans="1:3" x14ac:dyDescent="0.25">
@@ -21005,10 +21195,10 @@
         <v>2609</v>
       </c>
       <c r="B963" t="s">
-        <v>3291</v>
+        <v>3277</v>
       </c>
       <c r="C963" t="s">
-        <v>3292</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="964" spans="1:3" x14ac:dyDescent="0.25">
@@ -21016,10 +21206,10 @@
         <v>2610</v>
       </c>
       <c r="B964" t="s">
-        <v>3293</v>
+        <v>3279</v>
       </c>
       <c r="C964" t="s">
-        <v>3294</v>
+        <v>3280</v>
       </c>
     </row>
     <row r="965" spans="1:3" x14ac:dyDescent="0.25">
@@ -21126,10 +21316,10 @@
         <v>2638</v>
       </c>
       <c r="B974" t="s">
-        <v>3295</v>
+        <v>3281</v>
       </c>
       <c r="C974" t="s">
-        <v>3296</v>
+        <v>3282</v>
       </c>
     </row>
     <row r="975" spans="1:3" x14ac:dyDescent="0.25">
@@ -21137,10 +21327,10 @@
         <v>2639</v>
       </c>
       <c r="B975" t="s">
-        <v>3297</v>
+        <v>3283</v>
       </c>
       <c r="C975" t="s">
-        <v>3298</v>
+        <v>3284</v>
       </c>
     </row>
     <row r="976" spans="1:3" x14ac:dyDescent="0.25">
@@ -21192,10 +21382,10 @@
         <v>2652</v>
       </c>
       <c r="B980" t="s">
-        <v>3299</v>
+        <v>3285</v>
       </c>
       <c r="C980" t="s">
-        <v>3300</v>
+        <v>3286</v>
       </c>
     </row>
     <row r="981" spans="1:3" x14ac:dyDescent="0.25">
@@ -21236,10 +21426,10 @@
         <v>2661</v>
       </c>
       <c r="B984" t="s">
-        <v>3301</v>
+        <v>3287</v>
       </c>
       <c r="C984" t="s">
-        <v>3302</v>
+        <v>3288</v>
       </c>
     </row>
     <row r="985" spans="1:3" x14ac:dyDescent="0.25">
@@ -21335,10 +21525,10 @@
         <v>2686</v>
       </c>
       <c r="B993" t="s">
-        <v>3303</v>
+        <v>3289</v>
       </c>
       <c r="C993" t="s">
-        <v>3304</v>
+        <v>3290</v>
       </c>
     </row>
     <row r="994" spans="1:3" x14ac:dyDescent="0.25">
@@ -21808,10 +21998,10 @@
         <v>2809</v>
       </c>
       <c r="B1036" t="s">
-        <v>3305</v>
+        <v>3291</v>
       </c>
       <c r="C1036" t="s">
-        <v>3306</v>
+        <v>3292</v>
       </c>
     </row>
     <row r="1037" spans="1:3" x14ac:dyDescent="0.25">
@@ -22094,10 +22284,10 @@
         <v>2885</v>
       </c>
       <c r="B1062" t="s">
-        <v>3307</v>
+        <v>3293</v>
       </c>
       <c r="C1062" t="s">
-        <v>3308</v>
+        <v>3294</v>
       </c>
     </row>
     <row r="1063" spans="1:3" x14ac:dyDescent="0.25">
@@ -22127,10 +22317,10 @@
         <v>2892</v>
       </c>
       <c r="B1065" t="s">
-        <v>3309</v>
+        <v>3295</v>
       </c>
       <c r="C1065" t="s">
-        <v>3310</v>
+        <v>3296</v>
       </c>
     </row>
     <row r="1066" spans="1:3" x14ac:dyDescent="0.25">
@@ -22424,10 +22614,10 @@
         <v>2971</v>
       </c>
       <c r="B1092" t="s">
-        <v>3311</v>
+        <v>3297</v>
       </c>
       <c r="C1092" t="s">
-        <v>3312</v>
+        <v>3298</v>
       </c>
     </row>
     <row r="1093" spans="1:3" x14ac:dyDescent="0.25">
@@ -22452,291 +22642,526 @@
         <v>2977</v>
       </c>
     </row>
-    <row r="1095" spans="1:3" ht="134.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1095" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1095" t="s">
+        <v>2978</v>
+      </c>
+      <c r="B1095" t="s">
+        <v>2979</v>
+      </c>
+      <c r="C1095" t="s">
+        <v>2980</v>
+      </c>
+    </row>
     <row r="1096" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1096" s="2" t="s">
-        <v>2980</v>
-      </c>
-      <c r="B1096" s="2" t="s">
+      <c r="A1096" t="s">
         <v>2981</v>
       </c>
-      <c r="C1096" s="2" t="s">
+      <c r="B1096" t="s">
         <v>2982</v>
       </c>
+      <c r="C1096" t="s">
+        <v>2983</v>
+      </c>
     </row>
     <row r="1097" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1097" s="2" t="s">
-        <v>2983</v>
-      </c>
-      <c r="B1097" s="2" t="s">
+      <c r="A1097" t="s">
         <v>2984</v>
       </c>
-      <c r="C1097" s="2" t="s">
+      <c r="B1097" t="s">
         <v>2985</v>
       </c>
+      <c r="C1097" t="s">
+        <v>2986</v>
+      </c>
     </row>
     <row r="1098" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1098" s="2" t="s">
-        <v>2986</v>
-      </c>
-      <c r="B1098" s="2" t="s">
+      <c r="A1098" t="s">
         <v>2987</v>
       </c>
-      <c r="C1098" s="2" t="s">
+      <c r="B1098" t="s">
         <v>2988</v>
       </c>
+      <c r="C1098" t="s">
+        <v>2989</v>
+      </c>
     </row>
     <row r="1099" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1099" s="2" t="s">
-        <v>2989</v>
-      </c>
-      <c r="B1099" s="2" t="s">
+      <c r="A1099" t="s">
         <v>2990</v>
       </c>
-      <c r="C1099" s="2" t="s">
+      <c r="B1099" t="s">
         <v>2991</v>
       </c>
+      <c r="C1099" t="s">
+        <v>2992</v>
+      </c>
     </row>
     <row r="1100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1100" s="2" t="s">
-        <v>2992</v>
-      </c>
-      <c r="B1100" s="2" t="s">
+      <c r="A1100" t="s">
         <v>2993</v>
       </c>
-      <c r="C1100" s="2" t="s">
+      <c r="B1100" t="s">
         <v>2994</v>
       </c>
+      <c r="C1100" t="s">
+        <v>2995</v>
+      </c>
     </row>
     <row r="1101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1101" s="2" t="s">
-        <v>2995</v>
-      </c>
-      <c r="B1101" s="2" t="s">
+      <c r="A1101" t="s">
+        <v>2996</v>
+      </c>
+      <c r="B1101" t="s">
+        <v>3299</v>
+      </c>
+      <c r="C1101" t="s">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1102" t="s">
+        <v>2997</v>
+      </c>
+      <c r="B1102" t="s">
+        <v>2998</v>
+      </c>
+      <c r="C1102" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1103" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B1103" t="s">
+        <v>3001</v>
+      </c>
+      <c r="C1103" t="s">
+        <v>3002</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1104" t="s">
+        <v>3003</v>
+      </c>
+      <c r="B1104" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C1104" t="s">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1105" t="s">
+        <v>3006</v>
+      </c>
+      <c r="B1105" t="s">
+        <v>3301</v>
+      </c>
+      <c r="C1105" t="s">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1106" t="s">
+        <v>3007</v>
+      </c>
+      <c r="B1106" t="s">
+        <v>3008</v>
+      </c>
+      <c r="C1106" t="s">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1107" t="s">
+        <v>3010</v>
+      </c>
+      <c r="B1107" t="s">
+        <v>3011</v>
+      </c>
+      <c r="C1107" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1108" t="s">
+        <v>3013</v>
+      </c>
+      <c r="B1108" t="s">
+        <v>3014</v>
+      </c>
+      <c r="C1108" t="s">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1109" t="s">
+        <v>3016</v>
+      </c>
+      <c r="B1109" t="s">
+        <v>3017</v>
+      </c>
+      <c r="C1109" t="s">
+        <v>3018</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1110" t="s">
+        <v>3019</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>3020</v>
+      </c>
+      <c r="C1110" t="s">
+        <v>3021</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1111" t="s">
+        <v>3022</v>
+      </c>
+      <c r="B1111" t="s">
+        <v>3023</v>
+      </c>
+      <c r="C1111" t="s">
+        <v>3024</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1112" t="s">
+        <v>3025</v>
+      </c>
+      <c r="B1112" t="s">
+        <v>3026</v>
+      </c>
+      <c r="C1112" t="s">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1113" t="s">
+        <v>3028</v>
+      </c>
+      <c r="B1113" t="s">
+        <v>3029</v>
+      </c>
+      <c r="C1113" t="s">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1114" t="s">
+        <v>3031</v>
+      </c>
+      <c r="B1114" t="s">
+        <v>3032</v>
+      </c>
+      <c r="C1114" t="s">
+        <v>3033</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1115" t="s">
+        <v>3034</v>
+      </c>
+      <c r="B1115" t="s">
+        <v>3035</v>
+      </c>
+      <c r="C1115" t="s">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:3" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1116" s="2"/>
+      <c r="B1116" s="2"/>
+      <c r="C1116" s="2"/>
+    </row>
+    <row r="1117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1117" s="4" t="s">
+        <v>3305</v>
+      </c>
+      <c r="B1117" s="4" t="s">
+        <v>3306</v>
+      </c>
+      <c r="C1117" s="4" t="s">
+        <v>3307</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1118" s="4" t="s">
+        <v>3308</v>
+      </c>
+      <c r="B1118" s="4" t="s">
+        <v>3309</v>
+      </c>
+      <c r="C1118" s="4" t="s">
+        <v>3310</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1119" s="4" t="s">
+        <v>3311</v>
+      </c>
+      <c r="B1119" s="4" t="s">
+        <v>3312</v>
+      </c>
+      <c r="C1119" s="4" t="s">
         <v>3313</v>
       </c>
-      <c r="C1101" s="2" t="s">
+    </row>
+    <row r="1120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1120" s="4" t="s">
+        <v>3314</v>
+      </c>
+      <c r="B1120" s="4" t="s">
         <v>3315</v>
       </c>
-    </row>
-    <row r="1102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1102" s="2" t="s">
-        <v>2996</v>
-      </c>
-      <c r="B1102" s="3" t="s">
-        <v>2997</v>
-      </c>
-      <c r="C1102" s="2" t="s">
-        <v>2998</v>
-      </c>
-    </row>
-    <row r="1103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1103" s="2" t="s">
-        <v>2999</v>
-      </c>
-      <c r="B1103" s="3" t="s">
-        <v>3000</v>
-      </c>
-      <c r="C1103" s="2" t="s">
-        <v>3001</v>
-      </c>
-    </row>
-    <row r="1104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1104" s="2" t="s">
-        <v>3002</v>
-      </c>
-      <c r="B1104" s="2" t="s">
-        <v>3314</v>
-      </c>
-      <c r="C1104" s="2" t="s">
+      <c r="C1120" s="4" t="s">
         <v>3316</v>
       </c>
     </row>
-    <row r="1105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1105" s="3" t="s">
-        <v>3003</v>
-      </c>
-      <c r="B1105" s="2" t="s">
+    <row r="1121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1121" s="4" t="s">
+        <v>3317</v>
+      </c>
+      <c r="B1121" s="4" t="s">
+        <v>3318</v>
+      </c>
+      <c r="C1121" s="4" t="s">
+        <v>3319</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1122" s="4" t="s">
+        <v>3320</v>
+      </c>
+      <c r="B1122" s="4" t="s">
+        <v>3321</v>
+      </c>
+      <c r="C1122" s="4" t="s">
+        <v>3322</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1123" s="4" t="s">
+        <v>3323</v>
+      </c>
+      <c r="B1123" s="5" t="s">
+        <v>3324</v>
+      </c>
+      <c r="C1123" s="4" t="s">
+        <v>3325</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1124" s="4" t="s">
+        <v>3326</v>
+      </c>
+      <c r="B1124" s="5" t="s">
+        <v>3327</v>
+      </c>
+      <c r="C1124" s="4" t="s">
+        <v>3328</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1125" s="4" t="s">
+        <v>3329</v>
+      </c>
+      <c r="B1125" s="4" t="s">
+        <v>3330</v>
+      </c>
+      <c r="C1125" s="4" t="s">
+        <v>3331</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1126" s="5" t="s">
+        <v>3332</v>
+      </c>
+      <c r="B1126" s="4" t="s">
         <v>821</v>
       </c>
-      <c r="C1105" s="2" t="s">
-        <v>3004</v>
-      </c>
-    </row>
-    <row r="1106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1106" s="2" t="s">
-        <v>3005</v>
-      </c>
-      <c r="B1106" s="2" t="s">
-        <v>3006</v>
-      </c>
-      <c r="C1106" s="2" t="s">
-        <v>3007</v>
-      </c>
-    </row>
-    <row r="1107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1107" s="4" t="s">
+      <c r="C1126" s="4" t="s">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1127" s="4" t="s">
+        <v>3334</v>
+      </c>
+      <c r="B1127" s="4" t="s">
+        <v>3335</v>
+      </c>
+      <c r="C1127" s="4" t="s">
+        <v>3336</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1128" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="B1107" s="4" t="s">
-        <v>3008</v>
-      </c>
-      <c r="C1107" s="5" t="s">
-        <v>3009</v>
-      </c>
-    </row>
-    <row r="1108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1108" s="4" t="s">
-        <v>3010</v>
-      </c>
-      <c r="B1108" s="4" t="s">
-        <v>3011</v>
-      </c>
-      <c r="C1108" s="5" t="s">
-        <v>3012</v>
-      </c>
-    </row>
-    <row r="1109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1109" s="5" t="s">
-        <v>3013</v>
-      </c>
-      <c r="B1109" s="2" t="s">
-        <v>3014</v>
-      </c>
-      <c r="C1109" s="2" t="s">
-        <v>3015</v>
-      </c>
-    </row>
-    <row r="1110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1110" s="5" t="s">
-        <v>3016</v>
-      </c>
-      <c r="B1110" s="6" t="s">
-        <v>3017</v>
-      </c>
-      <c r="C1110" s="5" t="s">
-        <v>3018</v>
-      </c>
-    </row>
-    <row r="1111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1111" s="1" t="s">
-        <v>3019</v>
-      </c>
-      <c r="B1111" s="1" t="s">
-        <v>3020</v>
-      </c>
-      <c r="C1111" s="1" t="s">
-        <v>3021</v>
-      </c>
-    </row>
-    <row r="1112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1112" s="1" t="s">
-        <v>3022</v>
-      </c>
-      <c r="B1112" s="1" t="s">
-        <v>3023</v>
-      </c>
-      <c r="C1112" s="1" t="s">
-        <v>3024</v>
-      </c>
-    </row>
-    <row r="1113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1113" s="1" t="s">
-        <v>3025</v>
-      </c>
-      <c r="B1113" s="1" t="s">
-        <v>3026</v>
-      </c>
-      <c r="C1113" s="1" t="s">
-        <v>3027</v>
-      </c>
-    </row>
-    <row r="1114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1114" s="1" t="s">
-        <v>3028</v>
-      </c>
-      <c r="B1114" s="1" t="s">
-        <v>3029</v>
-      </c>
-      <c r="C1114" s="1" t="s">
-        <v>3030</v>
-      </c>
-    </row>
-    <row r="1115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1115" s="1" t="s">
-        <v>3031</v>
-      </c>
-      <c r="B1115" s="1" t="s">
-        <v>3032</v>
-      </c>
-      <c r="C1115" s="1" t="s">
-        <v>3033</v>
-      </c>
-    </row>
-    <row r="1116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1116" s="1" t="s">
-        <v>3034</v>
-      </c>
-      <c r="B1116" s="1" t="s">
-        <v>3035</v>
-      </c>
-      <c r="C1116" s="1" t="s">
-        <v>3036</v>
-      </c>
-    </row>
-    <row r="1117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1117" s="1" t="s">
-        <v>3037</v>
-      </c>
-      <c r="B1117" s="1" t="s">
+      <c r="B1128" s="6" t="s">
+        <v>3337</v>
+      </c>
+      <c r="C1128" s="7" t="s">
+        <v>3338</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1129" s="6" t="s">
+        <v>3339</v>
+      </c>
+      <c r="B1129" s="6" t="s">
+        <v>3340</v>
+      </c>
+      <c r="C1129" s="7" t="s">
+        <v>3341</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1130" s="7" t="s">
+        <v>3342</v>
+      </c>
+      <c r="B1130" s="4" t="s">
+        <v>3343</v>
+      </c>
+      <c r="C1130" s="4" t="s">
+        <v>3344</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1131" s="7" t="s">
+        <v>3345</v>
+      </c>
+      <c r="B1131" s="8" t="s">
+        <v>3346</v>
+      </c>
+      <c r="C1131" s="7" t="s">
+        <v>3347</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1132" s="3" t="s">
+        <v>3348</v>
+      </c>
+      <c r="B1132" s="3" t="s">
+        <v>3349</v>
+      </c>
+      <c r="C1132" s="3" t="s">
+        <v>3350</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1133" s="3" t="s">
+        <v>3351</v>
+      </c>
+      <c r="B1133" s="3" t="s">
+        <v>3352</v>
+      </c>
+      <c r="C1133" s="3" t="s">
+        <v>3353</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1134" s="3" t="s">
+        <v>3354</v>
+      </c>
+      <c r="B1134" s="3" t="s">
+        <v>3355</v>
+      </c>
+      <c r="C1134" s="3" t="s">
+        <v>3356</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1135" s="3" t="s">
+        <v>3357</v>
+      </c>
+      <c r="B1135" s="3" t="s">
+        <v>3358</v>
+      </c>
+      <c r="C1135" s="3" t="s">
+        <v>3359</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1136" s="3" t="s">
+        <v>3360</v>
+      </c>
+      <c r="B1136" s="3" t="s">
+        <v>3361</v>
+      </c>
+      <c r="C1136" s="3" t="s">
+        <v>3362</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1137" s="3" t="s">
+        <v>3363</v>
+      </c>
+      <c r="B1137" s="3" t="s">
+        <v>3364</v>
+      </c>
+      <c r="C1137" s="3" t="s">
+        <v>3365</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1138" s="3" t="s">
+        <v>3366</v>
+      </c>
+      <c r="B1138" s="3" t="s">
         <v>998</v>
       </c>
-      <c r="C1117" s="1" t="s">
+      <c r="C1138" s="3" t="s">
         <v>1129</v>
       </c>
     </row>
-    <row r="1118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1118" s="1" t="s">
-        <v>3038</v>
-      </c>
-      <c r="B1118" s="1" t="s">
-        <v>3039</v>
-      </c>
-      <c r="C1118" s="1" t="s">
-        <v>3040</v>
-      </c>
-    </row>
-    <row r="1119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1119" s="1" t="s">
-        <v>3041</v>
-      </c>
-      <c r="B1119" s="1" t="s">
-        <v>3042</v>
-      </c>
-      <c r="C1119" s="1" t="s">
-        <v>3043</v>
-      </c>
-    </row>
-    <row r="1120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1120" s="1" t="s">
-        <v>3044</v>
-      </c>
-      <c r="B1120" s="1" t="s">
-        <v>3045</v>
-      </c>
-      <c r="C1120" s="1" t="s">
-        <v>3046</v>
-      </c>
-    </row>
-    <row r="1121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1121" s="1" t="s">
-        <v>3047</v>
-      </c>
-      <c r="B1121" s="5" t="s">
-        <v>3048</v>
-      </c>
-      <c r="C1121" s="5" t="s">
-        <v>3049</v>
+    <row r="1139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1139" s="3" t="s">
+        <v>3367</v>
+      </c>
+      <c r="B1139" s="3" t="s">
+        <v>3368</v>
+      </c>
+      <c r="C1139" s="3" t="s">
+        <v>3369</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1140" s="3" t="s">
+        <v>3370</v>
+      </c>
+      <c r="B1140" s="3" t="s">
+        <v>3371</v>
+      </c>
+      <c r="C1140" s="3" t="s">
+        <v>3372</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1141" s="3" t="s">
+        <v>3373</v>
+      </c>
+      <c r="B1141" s="3" t="s">
+        <v>3374</v>
+      </c>
+      <c r="C1141" s="3" t="s">
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1142" s="3" t="s">
+        <v>3376</v>
+      </c>
+      <c r="B1142" s="7" t="s">
+        <v>3377</v>
+      </c>
+      <c r="C1142" s="7" t="s">
+        <v>3378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WebClient - a couple of ReturnCode localization strings
</commit_message>
<xml_diff>
--- a/Client/WebClient/lang/fibertest_strings.xlsx
+++ b/Client/WebClient/lang/fibertest_strings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VsGitProjects\Fibertest20\Client\WebClient\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516A1E2D-C698-42D1-A766-A9A162346BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EBEF2D-198C-4D1E-AA8C-40C399B82BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10630,7 +10630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -10649,9 +10649,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10998,15 +10995,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A1156" workbookViewId="0">
+      <selection activeCell="A1167" sqref="A1167:XFD1167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="97" customWidth="1"/>
-    <col min="2" max="2" width="120.28515625" customWidth="1"/>
-    <col min="3" max="3" width="243.140625" customWidth="1"/>
+    <col min="1" max="1" width="67.7109375" customWidth="1"/>
+    <col min="2" max="2" width="77.42578125" customWidth="1"/>
+    <col min="3" max="3" width="93.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -23824,7 +23821,7 @@
         <v>3161</v>
       </c>
     </row>
-    <row r="1166" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1166" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1167" s="2" t="s">
         <v>3162</v>
@@ -23991,117 +23988,117 @@
       </c>
     </row>
     <row r="1182" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1182" s="7" t="s">
+      <c r="A1182" s="1" t="s">
         <v>3205</v>
       </c>
-      <c r="B1182" s="7" t="s">
+      <c r="B1182" s="1" t="s">
         <v>3206</v>
       </c>
-      <c r="C1182" s="7" t="s">
+      <c r="C1182" s="1" t="s">
         <v>3207</v>
       </c>
     </row>
     <row r="1183" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1183" s="7" t="s">
+      <c r="A1183" s="1" t="s">
         <v>3208</v>
       </c>
-      <c r="B1183" s="7" t="s">
+      <c r="B1183" s="1" t="s">
         <v>3209</v>
       </c>
-      <c r="C1183" s="7" t="s">
+      <c r="C1183" s="1" t="s">
         <v>3210</v>
       </c>
     </row>
     <row r="1184" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1184" s="7" t="s">
+      <c r="A1184" s="1" t="s">
         <v>3211</v>
       </c>
-      <c r="B1184" s="7" t="s">
+      <c r="B1184" s="1" t="s">
         <v>3212</v>
       </c>
-      <c r="C1184" s="7" t="s">
+      <c r="C1184" s="1" t="s">
         <v>3213</v>
       </c>
     </row>
     <row r="1185" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1185" s="7" t="s">
+      <c r="A1185" s="1" t="s">
         <v>3214</v>
       </c>
-      <c r="B1185" s="7" t="s">
+      <c r="B1185" s="1" t="s">
         <v>3215</v>
       </c>
-      <c r="C1185" s="7" t="s">
+      <c r="C1185" s="1" t="s">
         <v>3216</v>
       </c>
     </row>
     <row r="1186" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1186" s="7" t="s">
+      <c r="A1186" s="1" t="s">
         <v>3217</v>
       </c>
-      <c r="B1186" s="7" t="s">
+      <c r="B1186" s="1" t="s">
         <v>3218</v>
       </c>
-      <c r="C1186" s="7" t="s">
+      <c r="C1186" s="1" t="s">
         <v>3219</v>
       </c>
     </row>
     <row r="1187" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1187" s="7" t="s">
+      <c r="A1187" s="1" t="s">
         <v>3220</v>
       </c>
-      <c r="B1187" s="7" t="s">
+      <c r="B1187" s="1" t="s">
         <v>3221</v>
       </c>
-      <c r="C1187" s="7" t="s">
+      <c r="C1187" s="1" t="s">
         <v>3222</v>
       </c>
     </row>
     <row r="1188" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1188" s="7" t="s">
+      <c r="A1188" s="1" t="s">
         <v>3223</v>
       </c>
-      <c r="B1188" s="7" t="s">
+      <c r="B1188" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="C1188" s="7" t="s">
+      <c r="C1188" s="1" t="s">
         <v>1131</v>
       </c>
     </row>
     <row r="1189" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1189" s="7" t="s">
+      <c r="A1189" s="1" t="s">
         <v>3224</v>
       </c>
-      <c r="B1189" s="7" t="s">
+      <c r="B1189" s="1" t="s">
         <v>3225</v>
       </c>
-      <c r="C1189" s="7" t="s">
+      <c r="C1189" s="1" t="s">
         <v>3226</v>
       </c>
     </row>
     <row r="1190" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1190" s="7" t="s">
+      <c r="A1190" s="1" t="s">
         <v>3227</v>
       </c>
-      <c r="B1190" s="7" t="s">
+      <c r="B1190" s="1" t="s">
         <v>3228</v>
       </c>
-      <c r="C1190" s="7" t="s">
+      <c r="C1190" s="1" t="s">
         <v>3229</v>
       </c>
     </row>
     <row r="1191" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1191" s="7" t="s">
+      <c r="A1191" s="1" t="s">
         <v>3230</v>
       </c>
-      <c r="B1191" s="7" t="s">
+      <c r="B1191" s="1" t="s">
         <v>3231</v>
       </c>
-      <c r="C1191" s="7" t="s">
+      <c r="C1191" s="1" t="s">
         <v>3232</v>
       </c>
     </row>
     <row r="1192" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1192" s="7" t="s">
+      <c r="A1192" s="1" t="s">
         <v>3233</v>
       </c>
       <c r="B1192" s="5" t="s">

</xml_diff>